<commit_message>
Added remaining schema fields, pricing
</commit_message>
<xml_diff>
--- a/odcs-template.xlsx
+++ b/odcs-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonharrer/Projects/open-data-contract-standard-excel-template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jochen/Projects/open-data-contract-standard-excel-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FE1094-A6F3-6842-B397-A2E53C4765DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABE60BF-0163-E249-9B8D-D4F6E2434F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -33,17 +33,19 @@
     <definedName name="kind">Fundamentals!$C$4</definedName>
     <definedName name="name">Fundamentals!$C$8</definedName>
     <definedName name="owner">Fundamentals!$C$12</definedName>
+    <definedName name="priceAmount">Fundamentals!$C$24</definedName>
+    <definedName name="priceCurrency">Fundamentals!$C$25</definedName>
     <definedName name="schema.businessName" localSheetId="2">'Schema &lt;table_name&gt;'!$B$8</definedName>
     <definedName name="schema.dataGranularityDescription" localSheetId="2">'Schema &lt;table_name&gt;'!$B$10</definedName>
     <definedName name="schema.description" localSheetId="2">'Schema &lt;table_name&gt;'!$B$7</definedName>
     <definedName name="schema.name" localSheetId="2">'Schema &lt;table_name&gt;'!$B$5</definedName>
     <definedName name="schema.physicalName" localSheetId="2">'Schema &lt;table_name&gt;'!$B$9</definedName>
     <definedName name="schema.physicalType" localSheetId="2">'Schema &lt;table_name&gt;'!$B$6</definedName>
-    <definedName name="schema.properties" localSheetId="2">'Schema &lt;table_name&gt;'!$A$13:$M$1023</definedName>
+    <definedName name="schema.properties" localSheetId="2">'Schema &lt;table_name&gt;'!$A$13:$N$981</definedName>
     <definedName name="schema.tags" localSheetId="2">'Schema &lt;table_name&gt;'!$B$11</definedName>
     <definedName name="status">Fundamentals!$C$10</definedName>
     <definedName name="support">Support!$A$4:$F$1000</definedName>
-    <definedName name="tags">Fundamentals!$C$23</definedName>
+    <definedName name="tags">Fundamentals!$C$28</definedName>
     <definedName name="team">Team!$A$4:$G$1000</definedName>
     <definedName name="tenant">Fundamentals!$C$16</definedName>
     <definedName name="version">Fundamentals!$C$9</definedName>
@@ -65,8 +67,78 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="M13" authorId="0" shapeId="0" xr:uid="{713377E1-93A7-A947-B4A9-FEA269F346C5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Links to sources that provide more details on the element; examples would be a link to privacy statement, terms and conditions, license agreements, data catalog, or another tool.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Maps to first </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>authoritativeDefinitions.url</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N13" authorId="0" shapeId="0" xr:uid="{D9029396-B90F-AF44-AAAD-21D60275C274}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Type of definition for authority. Valid values are: businessDefinition, transformationImplementation, videoTutorial, tutorial, and implementation.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+ Maps to first authoritativeDefinitions.type</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="101">
   <si>
     <t>Property</t>
   </si>
@@ -120,9 +192,6 @@
   </si>
   <si>
     <t>table</t>
-  </si>
-  <si>
-    <t>Quality</t>
   </si>
   <si>
     <t>Schema</t>
@@ -287,13 +356,100 @@
   </si>
   <si>
     <t>Replaced By Username</t>
+  </si>
+  <si>
+    <t>Partitioned</t>
+  </si>
+  <si>
+    <t>Primary Key</t>
+  </si>
+  <si>
+    <t>Primary Key Position</t>
+  </si>
+  <si>
+    <t>Partition Key Position</t>
+  </si>
+  <si>
+    <t>Encrypted Name</t>
+  </si>
+  <si>
+    <t>Transform Sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform Logic	</t>
+  </si>
+  <si>
+    <t>Transform Description</t>
+  </si>
+  <si>
+    <t>Critical Data Element Status</t>
+  </si>
+  <si>
+    <t>Maximum Items</t>
+  </si>
+  <si>
+    <t>Logical Type Options</t>
+  </si>
+  <si>
+    <t>Minimum Items</t>
+  </si>
+  <si>
+    <t>Unique Items</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Exclusive Maximum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Exclusice Minimum</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Multiple Of</t>
+  </si>
+  <si>
+    <t>Maximum Properties</t>
+  </si>
+  <si>
+    <t>Minimum Properties</t>
+  </si>
+  <si>
+    <t>Required (Object)</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>Quality Description</t>
+  </si>
+  <si>
+    <t>Quality Type</t>
+  </si>
+  <si>
+    <t>Pricing</t>
+  </si>
+  <si>
+    <t>Price Amount</t>
+  </si>
+  <si>
+    <t>Price Currency</t>
+  </si>
+  <si>
+    <t>Price Unit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,8 +495,21 @@
       <color rgb="FF000000"/>
       <name val="Aptos"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,8 +540,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCBD5E1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -454,11 +629,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -522,6 +728,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,9 +745,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD1D5DB"/>
+      <color rgb="FFCBD5E1"/>
       <color rgb="FF64748B"/>
       <color rgb="FFF3F4F6"/>
-      <color rgb="FFD1D5DB"/>
     </mruColors>
   </colors>
   <extLst>
@@ -888,7 +1104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -898,7 +1114,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -907,7 +1123,7 @@
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -923,7 +1139,7 @@
     </row>
     <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -936,7 +1152,7 @@
     </row>
     <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -949,7 +1165,7 @@
     </row>
     <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -962,7 +1178,7 @@
     </row>
     <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -975,7 +1191,7 @@
     </row>
     <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -1021,7 +1237,7 @@
     </row>
     <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1034,7 +1250,7 @@
     </row>
     <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -1047,7 +1263,7 @@
     </row>
     <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -1060,7 +1276,7 @@
     </row>
     <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -1073,7 +1289,7 @@
     </row>
     <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -1163,10 +1379,10 @@
     </row>
     <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>42</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>43</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -1178,10 +1394,10 @@
     </row>
     <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>41</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -1193,10 +1409,10 @@
     </row>
     <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="13" t="s">
         <v>44</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>45</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -1247,10 +1463,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92ABE851-FB8B-2145-B7F8-5CF6722D55A6}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1271,17 +1487,17 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="5" t="s">
@@ -1303,7 +1519,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="5"/>
@@ -1317,14 +1533,14 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
@@ -1335,7 +1551,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="5"/>
@@ -1347,7 +1563,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="5"/>
@@ -1355,7 +1571,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="5"/>
@@ -1363,7 +1579,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="5"/>
@@ -1381,21 +1597,21 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="5"/>
     </row>
@@ -1405,24 +1621,51 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="5"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="5"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A12:B12"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="G17:L27 G11:L13" xr:uid="{7EB39568-B879-514E-B51D-6C44C6D6A95F}">
+    <dataValidation type="list" allowBlank="1" sqref="G11:L13 G28:L29 G17:L22 G23:L26" xr:uid="{7EB39568-B879-514E-B51D-6C44C6D6A95F}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D22 D24:D27 D17:D18 D11:D13" xr:uid="{1D2456BD-0546-F940-A9EF-51615EED43D0}">
+    <dataValidation type="list" allowBlank="1" sqref="D22 D17:D18 D11:D13 D29 D23" xr:uid="{1D2456BD-0546-F940-A9EF-51615EED43D0}">
       <formula1>"string,number,integer,boolean,array,object"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Owner" prompt="The ID of the team owning the Data Contract._x000a_Required for Data Mesh Manager." sqref="C12" xr:uid="{35986E89-F1AF-D84C-96AD-8E5AC4A64A86}"/>
-    <dataValidation allowBlank="1" sqref="C24:C75 C17:C18 C22 C11:C13" xr:uid="{D875F021-2666-244F-B1D7-40151775E3CC}"/>
+    <dataValidation allowBlank="1" sqref="C11:C13 C17:C18 C22 C27:C70 C23" xr:uid="{D875F021-2666-244F-B1D7-40151775E3CC}"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1430,14 +1673,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AK49"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="24" style="2" bestFit="1" customWidth="1"/>
@@ -1447,42 +1688,49 @@
     <col min="6" max="6" width="35.6640625" style="2" customWidth="1"/>
     <col min="7" max="8" width="10" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="25.83203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="28.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="2"/>
+    <col min="10" max="11" width="14.33203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="25.83203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="28.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="22" width="19" style="2" customWidth="1"/>
+    <col min="23" max="23" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="37" width="21.6640625" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="38" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>17</v>
@@ -1491,7 +1739,7 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -1500,7 +1748,7 @@
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -1509,25 +1757,25 @@
       <c r="D8" s="23"/>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="22"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -1536,7 +1784,24 @@
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Y12" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z12" s="26"/>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="26"/>
+      <c r="AC12" s="26"/>
+      <c r="AD12" s="26"/>
+      <c r="AE12" s="26"/>
+      <c r="AF12" s="26"/>
+      <c r="AG12" s="26"/>
+      <c r="AH12" s="26"/>
+      <c r="AI12" s="26"/>
+      <c r="AJ12" s="26"/>
+      <c r="AK12" s="27"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>0</v>
       </c>
@@ -1568,16 +1833,88 @@
         <v>13</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="L13" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="M13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="M13" s="10" t="s">
+      <c r="N13" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="R13" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="S13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="T13" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="U13" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="V13" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="W13" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="X13" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y13" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z13" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA13" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB13" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC13" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD13" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE13" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG13" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH13" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AI13" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ13" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AK13" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -1591,8 +1928,32 @@
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15"/>
+      <c r="AF14" s="15"/>
+      <c r="AG14" s="15"/>
+      <c r="AH14" s="15"/>
+      <c r="AI14" s="15"/>
+      <c r="AJ14" s="15"/>
+      <c r="AK14" s="15"/>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1606,8 +1967,32 @@
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="15"/>
+      <c r="AF15" s="15"/>
+      <c r="AG15" s="15"/>
+      <c r="AH15" s="15"/>
+      <c r="AI15" s="15"/>
+      <c r="AJ15" s="15"/>
+      <c r="AK15" s="15"/>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -1621,8 +2006,32 @@
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="15"/>
+      <c r="AD16" s="15"/>
+      <c r="AE16" s="15"/>
+      <c r="AF16" s="15"/>
+      <c r="AG16" s="15"/>
+      <c r="AH16" s="15"/>
+      <c r="AI16" s="15"/>
+      <c r="AJ16" s="15"/>
+      <c r="AK16" s="15"/>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -1636,8 +2045,32 @@
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+      <c r="AC17" s="15"/>
+      <c r="AD17" s="15"/>
+      <c r="AE17" s="15"/>
+      <c r="AF17" s="15"/>
+      <c r="AG17" s="15"/>
+      <c r="AH17" s="15"/>
+      <c r="AI17" s="15"/>
+      <c r="AJ17" s="15"/>
+      <c r="AK17" s="15"/>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -1651,8 +2084,32 @@
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
+      <c r="AC18" s="15"/>
+      <c r="AD18" s="15"/>
+      <c r="AE18" s="15"/>
+      <c r="AF18" s="15"/>
+      <c r="AG18" s="15"/>
+      <c r="AH18" s="15"/>
+      <c r="AI18" s="15"/>
+      <c r="AJ18" s="15"/>
+      <c r="AK18" s="15"/>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -1666,8 +2123,32 @@
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="15"/>
+      <c r="AC19" s="15"/>
+      <c r="AD19" s="15"/>
+      <c r="AE19" s="15"/>
+      <c r="AF19" s="15"/>
+      <c r="AG19" s="15"/>
+      <c r="AH19" s="15"/>
+      <c r="AI19" s="15"/>
+      <c r="AJ19" s="15"/>
+      <c r="AK19" s="15"/>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -1681,8 +2162,32 @@
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+      <c r="AC20" s="15"/>
+      <c r="AD20" s="15"/>
+      <c r="AE20" s="15"/>
+      <c r="AF20" s="15"/>
+      <c r="AG20" s="15"/>
+      <c r="AH20" s="15"/>
+      <c r="AI20" s="15"/>
+      <c r="AJ20" s="15"/>
+      <c r="AK20" s="15"/>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
@@ -1696,8 +2201,32 @@
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
+      <c r="AA21" s="15"/>
+      <c r="AB21" s="15"/>
+      <c r="AC21" s="15"/>
+      <c r="AD21" s="15"/>
+      <c r="AE21" s="15"/>
+      <c r="AF21" s="15"/>
+      <c r="AG21" s="15"/>
+      <c r="AH21" s="15"/>
+      <c r="AI21" s="15"/>
+      <c r="AJ21" s="15"/>
+      <c r="AK21" s="15"/>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -1711,8 +2240,32 @@
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+      <c r="AC22" s="15"/>
+      <c r="AD22" s="15"/>
+      <c r="AE22" s="15"/>
+      <c r="AF22" s="15"/>
+      <c r="AG22" s="15"/>
+      <c r="AH22" s="15"/>
+      <c r="AI22" s="15"/>
+      <c r="AJ22" s="15"/>
+      <c r="AK22" s="15"/>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -1726,8 +2279,32 @@
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="15"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
+      <c r="AC23" s="15"/>
+      <c r="AD23" s="15"/>
+      <c r="AE23" s="15"/>
+      <c r="AF23" s="15"/>
+      <c r="AG23" s="15"/>
+      <c r="AH23" s="15"/>
+      <c r="AI23" s="15"/>
+      <c r="AJ23" s="15"/>
+      <c r="AK23" s="15"/>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -1741,8 +2318,32 @@
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="15"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+      <c r="AC24" s="15"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="15"/>
+      <c r="AF24" s="15"/>
+      <c r="AG24" s="15"/>
+      <c r="AH24" s="15"/>
+      <c r="AI24" s="15"/>
+      <c r="AJ24" s="15"/>
+      <c r="AK24" s="15"/>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -1756,8 +2357,32 @@
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
       <c r="M25" s="15"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="15"/>
+      <c r="W25" s="15"/>
+      <c r="X25" s="15"/>
+      <c r="Y25" s="15"/>
+      <c r="Z25" s="15"/>
+      <c r="AA25" s="15"/>
+      <c r="AB25" s="15"/>
+      <c r="AC25" s="15"/>
+      <c r="AD25" s="15"/>
+      <c r="AE25" s="15"/>
+      <c r="AF25" s="15"/>
+      <c r="AG25" s="15"/>
+      <c r="AH25" s="15"/>
+      <c r="AI25" s="15"/>
+      <c r="AJ25" s="15"/>
+      <c r="AK25" s="15"/>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -1771,8 +2396,32 @@
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
       <c r="M26" s="15"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="15"/>
+      <c r="X26" s="15"/>
+      <c r="Y26" s="15"/>
+      <c r="Z26" s="15"/>
+      <c r="AA26" s="15"/>
+      <c r="AB26" s="15"/>
+      <c r="AC26" s="15"/>
+      <c r="AD26" s="15"/>
+      <c r="AE26" s="15"/>
+      <c r="AF26" s="15"/>
+      <c r="AG26" s="15"/>
+      <c r="AH26" s="15"/>
+      <c r="AI26" s="15"/>
+      <c r="AJ26" s="15"/>
+      <c r="AK26" s="15"/>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -1786,8 +2435,32 @@
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
+      <c r="U27" s="15"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="15"/>
+      <c r="X27" s="15"/>
+      <c r="Y27" s="15"/>
+      <c r="Z27" s="15"/>
+      <c r="AA27" s="15"/>
+      <c r="AB27" s="15"/>
+      <c r="AC27" s="15"/>
+      <c r="AD27" s="15"/>
+      <c r="AE27" s="15"/>
+      <c r="AF27" s="15"/>
+      <c r="AG27" s="15"/>
+      <c r="AH27" s="15"/>
+      <c r="AI27" s="15"/>
+      <c r="AJ27" s="15"/>
+      <c r="AK27" s="15"/>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1801,8 +2474,32 @@
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="15"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="15"/>
+      <c r="Y28" s="15"/>
+      <c r="Z28" s="15"/>
+      <c r="AA28" s="15"/>
+      <c r="AB28" s="15"/>
+      <c r="AC28" s="15"/>
+      <c r="AD28" s="15"/>
+      <c r="AE28" s="15"/>
+      <c r="AF28" s="15"/>
+      <c r="AG28" s="15"/>
+      <c r="AH28" s="15"/>
+      <c r="AI28" s="15"/>
+      <c r="AJ28" s="15"/>
+      <c r="AK28" s="15"/>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1816,8 +2513,32 @@
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
       <c r="M29" s="15"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="15"/>
+      <c r="U29" s="15"/>
+      <c r="V29" s="15"/>
+      <c r="W29" s="15"/>
+      <c r="X29" s="15"/>
+      <c r="Y29" s="15"/>
+      <c r="Z29" s="15"/>
+      <c r="AA29" s="15"/>
+      <c r="AB29" s="15"/>
+      <c r="AC29" s="15"/>
+      <c r="AD29" s="15"/>
+      <c r="AE29" s="15"/>
+      <c r="AF29" s="15"/>
+      <c r="AG29" s="15"/>
+      <c r="AH29" s="15"/>
+      <c r="AI29" s="15"/>
+      <c r="AJ29" s="15"/>
+      <c r="AK29" s="15"/>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1831,8 +2552,32 @@
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="15"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="15"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="15"/>
+      <c r="Z30" s="15"/>
+      <c r="AA30" s="15"/>
+      <c r="AB30" s="15"/>
+      <c r="AC30" s="15"/>
+      <c r="AD30" s="15"/>
+      <c r="AE30" s="15"/>
+      <c r="AF30" s="15"/>
+      <c r="AG30" s="15"/>
+      <c r="AH30" s="15"/>
+      <c r="AI30" s="15"/>
+      <c r="AJ30" s="15"/>
+      <c r="AK30" s="15"/>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -1846,8 +2591,32 @@
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
       <c r="M31" s="15"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="15"/>
+      <c r="U31" s="15"/>
+      <c r="V31" s="15"/>
+      <c r="W31" s="15"/>
+      <c r="X31" s="15"/>
+      <c r="Y31" s="15"/>
+      <c r="Z31" s="15"/>
+      <c r="AA31" s="15"/>
+      <c r="AB31" s="15"/>
+      <c r="AC31" s="15"/>
+      <c r="AD31" s="15"/>
+      <c r="AE31" s="15"/>
+      <c r="AF31" s="15"/>
+      <c r="AG31" s="15"/>
+      <c r="AH31" s="15"/>
+      <c r="AI31" s="15"/>
+      <c r="AJ31" s="15"/>
+      <c r="AK31" s="15"/>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -1861,8 +2630,32 @@
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="15"/>
+      <c r="V32" s="15"/>
+      <c r="W32" s="15"/>
+      <c r="X32" s="15"/>
+      <c r="Y32" s="15"/>
+      <c r="Z32" s="15"/>
+      <c r="AA32" s="15"/>
+      <c r="AB32" s="15"/>
+      <c r="AC32" s="15"/>
+      <c r="AD32" s="15"/>
+      <c r="AE32" s="15"/>
+      <c r="AF32" s="15"/>
+      <c r="AG32" s="15"/>
+      <c r="AH32" s="15"/>
+      <c r="AI32" s="15"/>
+      <c r="AJ32" s="15"/>
+      <c r="AK32" s="15"/>
+    </row>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -1876,8 +2669,32 @@
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
       <c r="M33" s="15"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="15"/>
+      <c r="U33" s="15"/>
+      <c r="V33" s="15"/>
+      <c r="W33" s="15"/>
+      <c r="X33" s="15"/>
+      <c r="Y33" s="15"/>
+      <c r="Z33" s="15"/>
+      <c r="AA33" s="15"/>
+      <c r="AB33" s="15"/>
+      <c r="AC33" s="15"/>
+      <c r="AD33" s="15"/>
+      <c r="AE33" s="15"/>
+      <c r="AF33" s="15"/>
+      <c r="AG33" s="15"/>
+      <c r="AH33" s="15"/>
+      <c r="AI33" s="15"/>
+      <c r="AJ33" s="15"/>
+      <c r="AK33" s="15"/>
+    </row>
+    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -1891,8 +2708,32 @@
       <c r="K34" s="15"/>
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
+      <c r="T34" s="15"/>
+      <c r="U34" s="15"/>
+      <c r="V34" s="15"/>
+      <c r="W34" s="15"/>
+      <c r="X34" s="15"/>
+      <c r="Y34" s="15"/>
+      <c r="Z34" s="15"/>
+      <c r="AA34" s="15"/>
+      <c r="AB34" s="15"/>
+      <c r="AC34" s="15"/>
+      <c r="AD34" s="15"/>
+      <c r="AE34" s="15"/>
+      <c r="AF34" s="15"/>
+      <c r="AG34" s="15"/>
+      <c r="AH34" s="15"/>
+      <c r="AI34" s="15"/>
+      <c r="AJ34" s="15"/>
+      <c r="AK34" s="15"/>
+    </row>
+    <row r="35" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -1906,8 +2747,32 @@
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="15"/>
+      <c r="U35" s="15"/>
+      <c r="V35" s="15"/>
+      <c r="W35" s="15"/>
+      <c r="X35" s="15"/>
+      <c r="Y35" s="15"/>
+      <c r="Z35" s="15"/>
+      <c r="AA35" s="15"/>
+      <c r="AB35" s="15"/>
+      <c r="AC35" s="15"/>
+      <c r="AD35" s="15"/>
+      <c r="AE35" s="15"/>
+      <c r="AF35" s="15"/>
+      <c r="AG35" s="15"/>
+      <c r="AH35" s="15"/>
+      <c r="AI35" s="15"/>
+      <c r="AJ35" s="15"/>
+      <c r="AK35" s="15"/>
+    </row>
+    <row r="36" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -1921,8 +2786,32 @@
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="15"/>
+      <c r="U36" s="15"/>
+      <c r="V36" s="15"/>
+      <c r="W36" s="15"/>
+      <c r="X36" s="15"/>
+      <c r="Y36" s="15"/>
+      <c r="Z36" s="15"/>
+      <c r="AA36" s="15"/>
+      <c r="AB36" s="15"/>
+      <c r="AC36" s="15"/>
+      <c r="AD36" s="15"/>
+      <c r="AE36" s="15"/>
+      <c r="AF36" s="15"/>
+      <c r="AG36" s="15"/>
+      <c r="AH36" s="15"/>
+      <c r="AI36" s="15"/>
+      <c r="AJ36" s="15"/>
+      <c r="AK36" s="15"/>
+    </row>
+    <row r="37" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -1936,8 +2825,32 @@
       <c r="K37" s="15"/>
       <c r="L37" s="15"/>
       <c r="M37" s="15"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+      <c r="V37" s="15"/>
+      <c r="W37" s="15"/>
+      <c r="X37" s="15"/>
+      <c r="Y37" s="15"/>
+      <c r="Z37" s="15"/>
+      <c r="AA37" s="15"/>
+      <c r="AB37" s="15"/>
+      <c r="AC37" s="15"/>
+      <c r="AD37" s="15"/>
+      <c r="AE37" s="15"/>
+      <c r="AF37" s="15"/>
+      <c r="AG37" s="15"/>
+      <c r="AH37" s="15"/>
+      <c r="AI37" s="15"/>
+      <c r="AJ37" s="15"/>
+      <c r="AK37" s="15"/>
+    </row>
+    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -1951,8 +2864,32 @@
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="15"/>
+      <c r="V38" s="15"/>
+      <c r="W38" s="15"/>
+      <c r="X38" s="15"/>
+      <c r="Y38" s="15"/>
+      <c r="Z38" s="15"/>
+      <c r="AA38" s="15"/>
+      <c r="AB38" s="15"/>
+      <c r="AC38" s="15"/>
+      <c r="AD38" s="15"/>
+      <c r="AE38" s="15"/>
+      <c r="AF38" s="15"/>
+      <c r="AG38" s="15"/>
+      <c r="AH38" s="15"/>
+      <c r="AI38" s="15"/>
+      <c r="AJ38" s="15"/>
+      <c r="AK38" s="15"/>
+    </row>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -1966,8 +2903,32 @@
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="15"/>
+      <c r="S39" s="15"/>
+      <c r="T39" s="15"/>
+      <c r="U39" s="15"/>
+      <c r="V39" s="15"/>
+      <c r="W39" s="15"/>
+      <c r="X39" s="15"/>
+      <c r="Y39" s="15"/>
+      <c r="Z39" s="15"/>
+      <c r="AA39" s="15"/>
+      <c r="AB39" s="15"/>
+      <c r="AC39" s="15"/>
+      <c r="AD39" s="15"/>
+      <c r="AE39" s="15"/>
+      <c r="AF39" s="15"/>
+      <c r="AG39" s="15"/>
+      <c r="AH39" s="15"/>
+      <c r="AI39" s="15"/>
+      <c r="AJ39" s="15"/>
+      <c r="AK39" s="15"/>
+    </row>
+    <row r="40" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -1981,8 +2942,32 @@
       <c r="K40" s="15"/>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="15"/>
+      <c r="V40" s="15"/>
+      <c r="W40" s="15"/>
+      <c r="X40" s="15"/>
+      <c r="Y40" s="15"/>
+      <c r="Z40" s="15"/>
+      <c r="AA40" s="15"/>
+      <c r="AB40" s="15"/>
+      <c r="AC40" s="15"/>
+      <c r="AD40" s="15"/>
+      <c r="AE40" s="15"/>
+      <c r="AF40" s="15"/>
+      <c r="AG40" s="15"/>
+      <c r="AH40" s="15"/>
+      <c r="AI40" s="15"/>
+      <c r="AJ40" s="15"/>
+      <c r="AK40" s="15"/>
+    </row>
+    <row r="41" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -1996,8 +2981,32 @@
       <c r="K41" s="15"/>
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
+      <c r="S41" s="15"/>
+      <c r="T41" s="15"/>
+      <c r="U41" s="15"/>
+      <c r="V41" s="15"/>
+      <c r="W41" s="15"/>
+      <c r="X41" s="15"/>
+      <c r="Y41" s="15"/>
+      <c r="Z41" s="15"/>
+      <c r="AA41" s="15"/>
+      <c r="AB41" s="15"/>
+      <c r="AC41" s="15"/>
+      <c r="AD41" s="15"/>
+      <c r="AE41" s="15"/>
+      <c r="AF41" s="15"/>
+      <c r="AG41" s="15"/>
+      <c r="AH41" s="15"/>
+      <c r="AI41" s="15"/>
+      <c r="AJ41" s="15"/>
+      <c r="AK41" s="15"/>
+    </row>
+    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -2011,8 +3020,32 @@
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="15"/>
+      <c r="T42" s="15"/>
+      <c r="U42" s="15"/>
+      <c r="V42" s="15"/>
+      <c r="W42" s="15"/>
+      <c r="X42" s="15"/>
+      <c r="Y42" s="15"/>
+      <c r="Z42" s="15"/>
+      <c r="AA42" s="15"/>
+      <c r="AB42" s="15"/>
+      <c r="AC42" s="15"/>
+      <c r="AD42" s="15"/>
+      <c r="AE42" s="15"/>
+      <c r="AF42" s="15"/>
+      <c r="AG42" s="15"/>
+      <c r="AH42" s="15"/>
+      <c r="AI42" s="15"/>
+      <c r="AJ42" s="15"/>
+      <c r="AK42" s="15"/>
+    </row>
+    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -2026,8 +3059,32 @@
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="15"/>
+      <c r="T43" s="15"/>
+      <c r="U43" s="15"/>
+      <c r="V43" s="15"/>
+      <c r="W43" s="15"/>
+      <c r="X43" s="15"/>
+      <c r="Y43" s="15"/>
+      <c r="Z43" s="15"/>
+      <c r="AA43" s="15"/>
+      <c r="AB43" s="15"/>
+      <c r="AC43" s="15"/>
+      <c r="AD43" s="15"/>
+      <c r="AE43" s="15"/>
+      <c r="AF43" s="15"/>
+      <c r="AG43" s="15"/>
+      <c r="AH43" s="15"/>
+      <c r="AI43" s="15"/>
+      <c r="AJ43" s="15"/>
+      <c r="AK43" s="15"/>
+    </row>
+    <row r="44" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -2041,8 +3098,32 @@
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="15"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="15"/>
+      <c r="X44" s="15"/>
+      <c r="Y44" s="15"/>
+      <c r="Z44" s="15"/>
+      <c r="AA44" s="15"/>
+      <c r="AB44" s="15"/>
+      <c r="AC44" s="15"/>
+      <c r="AD44" s="15"/>
+      <c r="AE44" s="15"/>
+      <c r="AF44" s="15"/>
+      <c r="AG44" s="15"/>
+      <c r="AH44" s="15"/>
+      <c r="AI44" s="15"/>
+      <c r="AJ44" s="15"/>
+      <c r="AK44" s="15"/>
+    </row>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -2056,8 +3137,32 @@
       <c r="K45" s="15"/>
       <c r="L45" s="15"/>
       <c r="M45" s="15"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
+      <c r="S45" s="15"/>
+      <c r="T45" s="15"/>
+      <c r="U45" s="15"/>
+      <c r="V45" s="15"/>
+      <c r="W45" s="15"/>
+      <c r="X45" s="15"/>
+      <c r="Y45" s="15"/>
+      <c r="Z45" s="15"/>
+      <c r="AA45" s="15"/>
+      <c r="AB45" s="15"/>
+      <c r="AC45" s="15"/>
+      <c r="AD45" s="15"/>
+      <c r="AE45" s="15"/>
+      <c r="AF45" s="15"/>
+      <c r="AG45" s="15"/>
+      <c r="AH45" s="15"/>
+      <c r="AI45" s="15"/>
+      <c r="AJ45" s="15"/>
+      <c r="AK45" s="15"/>
+    </row>
+    <row r="46" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -2071,8 +3176,32 @@
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+      <c r="R46" s="15"/>
+      <c r="S46" s="15"/>
+      <c r="T46" s="15"/>
+      <c r="U46" s="15"/>
+      <c r="V46" s="15"/>
+      <c r="W46" s="15"/>
+      <c r="X46" s="15"/>
+      <c r="Y46" s="15"/>
+      <c r="Z46" s="15"/>
+      <c r="AA46" s="15"/>
+      <c r="AB46" s="15"/>
+      <c r="AC46" s="15"/>
+      <c r="AD46" s="15"/>
+      <c r="AE46" s="15"/>
+      <c r="AF46" s="15"/>
+      <c r="AG46" s="15"/>
+      <c r="AH46" s="15"/>
+      <c r="AI46" s="15"/>
+      <c r="AJ46" s="15"/>
+      <c r="AK46" s="15"/>
+    </row>
+    <row r="47" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -2086,8 +3215,32 @@
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="15"/>
+      <c r="T47" s="15"/>
+      <c r="U47" s="15"/>
+      <c r="V47" s="15"/>
+      <c r="W47" s="15"/>
+      <c r="X47" s="15"/>
+      <c r="Y47" s="15"/>
+      <c r="Z47" s="15"/>
+      <c r="AA47" s="15"/>
+      <c r="AB47" s="15"/>
+      <c r="AC47" s="15"/>
+      <c r="AD47" s="15"/>
+      <c r="AE47" s="15"/>
+      <c r="AF47" s="15"/>
+      <c r="AG47" s="15"/>
+      <c r="AH47" s="15"/>
+      <c r="AI47" s="15"/>
+      <c r="AJ47" s="15"/>
+      <c r="AK47" s="15"/>
+    </row>
+    <row r="48" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -2101,8 +3254,32 @@
       <c r="K48" s="15"/>
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
+      <c r="S48" s="15"/>
+      <c r="T48" s="15"/>
+      <c r="U48" s="15"/>
+      <c r="V48" s="15"/>
+      <c r="W48" s="15"/>
+      <c r="X48" s="15"/>
+      <c r="Y48" s="15"/>
+      <c r="Z48" s="15"/>
+      <c r="AA48" s="15"/>
+      <c r="AB48" s="15"/>
+      <c r="AC48" s="15"/>
+      <c r="AD48" s="15"/>
+      <c r="AE48" s="15"/>
+      <c r="AF48" s="15"/>
+      <c r="AG48" s="15"/>
+      <c r="AH48" s="15"/>
+      <c r="AI48" s="15"/>
+      <c r="AJ48" s="15"/>
+      <c r="AK48" s="15"/>
+    </row>
+    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -2116,6 +3293,30 @@
       <c r="K49" s="15"/>
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
+      <c r="R49" s="15"/>
+      <c r="S49" s="15"/>
+      <c r="T49" s="15"/>
+      <c r="U49" s="15"/>
+      <c r="V49" s="15"/>
+      <c r="W49" s="15"/>
+      <c r="X49" s="15"/>
+      <c r="Y49" s="15"/>
+      <c r="Z49" s="15"/>
+      <c r="AA49" s="15"/>
+      <c r="AB49" s="15"/>
+      <c r="AC49" s="15"/>
+      <c r="AD49" s="15"/>
+      <c r="AE49" s="15"/>
+      <c r="AF49" s="15"/>
+      <c r="AG49" s="15"/>
+      <c r="AH49" s="15"/>
+      <c r="AI49" s="15"/>
+      <c r="AJ49" s="15"/>
+      <c r="AK49" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2127,22 +3328,32 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
   </mergeCells>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Unique" prompt="A value must be unique within the dataset" sqref="H14:H70" xr:uid="{274C493E-CBE0-2742-BFD6-A161E5736B5A}">
+  <dataValidations count="10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Unique" prompt="A value must be unique within the dataset" sqref="H14:H49" xr:uid="{274C493E-CBE0-2742-BFD6-A161E5736B5A}">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:C70" xr:uid="{792BC06D-75E6-1A4B-8EE7-26D8A0C4CF46}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:C49" xr:uid="{792BC06D-75E6-1A4B-8EE7-26D8A0C4CF46}">
       <formula1>"string,number,integer,boolean,array,object"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" sqref="B14:B70 L14:M70 I14:J70" xr:uid="{DDC4FF9F-5023-E04B-9FAD-8E0C431863DF}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Required" prompt="Is this a required field (true) or can it be optional (false)" sqref="G14:G70" xr:uid="{653181B6-028C-9348-B6A1-78F7EF7B9A52}">
+    <dataValidation allowBlank="1" sqref="B14:B49 O14:AK49 M14:M49 J14:J49" xr:uid="{DDC4FF9F-5023-E04B-9FAD-8E0C431863DF}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Required" prompt="Is this a required field (true) or can it be optional (false)" sqref="G14:G49" xr:uid="{653181B6-028C-9348-B6A1-78F7EF7B9A52}">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality" prompt="The expected or guaranteed data quality from a business perspective._x000a__x000a_Maps to quality.description" sqref="K14:K70" xr:uid="{7B1FC03E-550C-B248-B1C0-23683F595085}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality" prompt="The expected or guaranteed data quality from a business perspective._x000a__x000a_Maps to quality.description" sqref="L14:L49" xr:uid="{7B1FC03E-550C-B248-B1C0-23683F595085}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Schema Name" prompt="The name of the schema (e.g., table) must match the Sheet name &quot;Schema &lt;schema_name&gt;&quot;" sqref="B5:E5" xr:uid="{8B3F718D-6361-B845-86DC-2F310C7348A9}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Property" prompt="Name of the property._x000a_If you have structured objects (child properties), use the dot notation, e.g., address.street._x000a_If you have array structures, use the [] notation, e.g., credit_cards[].number." sqref="A13" xr:uid="{0D2C99EC-1C07-E24C-A3B9-1D3DE4A213B3}"/>
+    <dataValidation type="list" allowBlank="1" sqref="N14:N49" xr:uid="{B83703A8-BFB7-EA4A-8244-28C8F1668E20}">
+      <formula1>"businessDefinition,transformationImplementation,videoTutorial,tutorial,implementation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="I14:I49" xr:uid="{159197B4-47E7-9F48-923A-42F63EFB1F97}">
+      <formula1>"confidential,restricted,public"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="K14:K49" xr:uid="{B14CC525-9BD9-6A4D-BDFD-7963A22A4F85}">
+      <formula1>"text,library,sql,custom"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2164,32 +3375,32 @@
   <sheetData>
     <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>61</v>
-      </c>
       <c r="F4" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2340,7 +3551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD55E6DF-E5C5-C142-BA93-791862A30BE7}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2354,17 +3565,17 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>9</v>
@@ -2373,16 +3584,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="G4" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2563,12 +3774,12 @@
   <sheetData>
     <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2581,7 +3792,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="5" t="str">
         <f>IF(owner &lt;&gt; "", owner, "")</f>

</xml_diff>

<commit_message>
Update SLA Roles Servers
</commit_message>
<xml_diff>
--- a/odcs-template.xlsx
+++ b/odcs-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jochen/Projects/open-data-contract-standard-excel-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5B4C9E-94C4-914C-9F8B-42043AD11549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B01A6C5-0779-A544-9628-01F684BD1904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,11 @@
     <sheet name="Schema &lt;table_name&gt;" sheetId="3" r:id="rId3"/>
     <sheet name="Support" sheetId="12" r:id="rId4"/>
     <sheet name="Team" sheetId="13" r:id="rId5"/>
-    <sheet name="Pricing" sheetId="15" r:id="rId6"/>
-    <sheet name="Custom Properties" sheetId="11" r:id="rId7"/>
+    <sheet name="Roles" sheetId="16" r:id="rId6"/>
+    <sheet name="SLA" sheetId="17" r:id="rId7"/>
+    <sheet name="Servers" sheetId="20" r:id="rId8"/>
+    <sheet name="Pricing" sheetId="15" r:id="rId9"/>
+    <sheet name="Custom Properties" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="apiVersion">Fundamentals!$C$5</definedName>
@@ -37,6 +40,8 @@
     <definedName name="pricing.priceAmount">Pricing!$B$4</definedName>
     <definedName name="pricing.priceCurrency">Pricing!$B$5</definedName>
     <definedName name="pricing.priceUnit">Pricing!$B$6</definedName>
+    <definedName name="roles" localSheetId="5">Roles!$A$4:$E$1000</definedName>
+    <definedName name="roles" localSheetId="7">Servers!$A$4:$AE$982</definedName>
     <definedName name="schema.businessName" localSheetId="2">'Schema &lt;table_name&gt;'!$B$8</definedName>
     <definedName name="schema.dataGranularityDescription" localSheetId="2">'Schema &lt;table_name&gt;'!$B$10</definedName>
     <definedName name="schema.description" localSheetId="2">'Schema &lt;table_name&gt;'!$B$7</definedName>
@@ -45,6 +50,62 @@
     <definedName name="schema.physicalType" localSheetId="2">'Schema &lt;table_name&gt;'!$B$6</definedName>
     <definedName name="schema.properties" localSheetId="2">'Schema &lt;table_name&gt;'!$A$13:$N$981</definedName>
     <definedName name="schema.tags" localSheetId="2">'Schema &lt;table_name&gt;'!$B$11</definedName>
+    <definedName name="servers.azure.delimiter">Servers!$C$14</definedName>
+    <definedName name="servers.azure.format">Servers!$C$13</definedName>
+    <definedName name="servers.azure.location">Servers!$C$12</definedName>
+    <definedName name="servers.bigquery.dataset">Servers!$C$18</definedName>
+    <definedName name="servers.bigquery.project">Servers!$C$17</definedName>
+    <definedName name="servers.custom.account">Servers!$C$62</definedName>
+    <definedName name="servers.custom.catalog">Servers!$C$63</definedName>
+    <definedName name="servers.custom.database">Servers!$C$64</definedName>
+    <definedName name="servers.custom.dataset">Servers!$C$65</definedName>
+    <definedName name="servers.custom.delimiter">Servers!$C$66</definedName>
+    <definedName name="servers.custom.endpointUrl">Servers!$C$67</definedName>
+    <definedName name="servers.custom.format">Servers!$C$68</definedName>
+    <definedName name="servers.custom.host">Servers!$C$69</definedName>
+    <definedName name="servers.custom.location">Servers!$C$70</definedName>
+    <definedName name="servers.custom.path">Servers!$C$71</definedName>
+    <definedName name="servers.custom.port">Servers!$C$72</definedName>
+    <definedName name="servers.custom.project">Servers!$C$73</definedName>
+    <definedName name="servers.custom.region">Servers!$C$74</definedName>
+    <definedName name="servers.custom.regionName">Servers!$C$75</definedName>
+    <definedName name="servers.custom.schema">Servers!$C$76</definedName>
+    <definedName name="servers.custom.serviceName">Servers!$C$77</definedName>
+    <definedName name="servers.custom.stagingDirectory">Servers!$C$78</definedName>
+    <definedName name="servers.custom.stream">Servers!$C$79</definedName>
+    <definedName name="servers.custom.warehouse">Servers!$C$80</definedName>
+    <definedName name="servers.databricks.catalog">Servers!$C$21</definedName>
+    <definedName name="servers.databricks.host">Servers!$C$23</definedName>
+    <definedName name="servers.databricks.schema">Servers!$C$22</definedName>
+    <definedName name="servers.description">Servers!$C$6</definedName>
+    <definedName name="servers.environment">Servers!$C$5</definedName>
+    <definedName name="servers.glue.account">Servers!$C$26</definedName>
+    <definedName name="servers.glue.database">Servers!$C$27</definedName>
+    <definedName name="servers.glue.format">Servers!$C$29</definedName>
+    <definedName name="servers.glue.location">Servers!$C$28</definedName>
+    <definedName name="servers.kafka.format">Servers!$C$33</definedName>
+    <definedName name="servers.kafka.host">Servers!$C$32</definedName>
+    <definedName name="servers.postgres.database">Servers!$C$38</definedName>
+    <definedName name="servers.postgres.host">Servers!$C$36</definedName>
+    <definedName name="servers.postgres.port">Servers!$C$37</definedName>
+    <definedName name="servers.psotgres.schema">Servers!$C$39</definedName>
+    <definedName name="servers.s3.delimiter">Servers!$C$45</definedName>
+    <definedName name="servers.s3.endpointUrl">Servers!$C$43</definedName>
+    <definedName name="servers.s3.format">Servers!$C$44</definedName>
+    <definedName name="servers.s3.location">Servers!$C$42</definedName>
+    <definedName name="servers.server">Servers!$C$4</definedName>
+    <definedName name="servers.snowflake.account">Servers!$C$50</definedName>
+    <definedName name="servers.snowflake.database">Servers!$C$51</definedName>
+    <definedName name="servers.snowflake.host">Servers!$C$48</definedName>
+    <definedName name="servers.snowflake.port">Servers!$C$49</definedName>
+    <definedName name="servers.snowflake.schema">Servers!$C$53</definedName>
+    <definedName name="servers.snowflake.warehouse">Servers!$C$52</definedName>
+    <definedName name="servers.sqlserver.database">Servers!$C$58</definedName>
+    <definedName name="servers.sqlserver.host">Servers!$C$56</definedName>
+    <definedName name="servers.sqlserver.port">Servers!$C$57</definedName>
+    <definedName name="servers.sqlserver.schema">Servers!$C$59</definedName>
+    <definedName name="servers.type">Servers!$C$8</definedName>
+    <definedName name="slaProperties" localSheetId="6">SLA!$A$6:$F$1002</definedName>
     <definedName name="status">Fundamentals!$C$10</definedName>
     <definedName name="support">Support!$A$4:$F$1000</definedName>
     <definedName name="tags">Fundamentals!$C$23</definedName>
@@ -70,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="145">
   <si>
     <t>Property</t>
   </si>
@@ -379,6 +440,139 @@
   <si>
     <t xml:space="preserve">This section covers pricing when you bill your customer for using this data product.
 </t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This section lists team members and the history of their relation with this data contract.
+This section lists the roles that a consumer may need to access the dataset depending on the type of access they require.
+</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>1st Level Approvers</t>
+  </si>
+  <si>
+    <t>2nd Level Approvers</t>
+  </si>
+  <si>
+    <t>Service-Level Agreement (SLA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This section describes the service-level agreements (SLA).
+This section lists the roles that a consumer may need to access the dataset depending on the type of access they require.
+</t>
+  </si>
+  <si>
+    <t>Default SLA element(s)</t>
+  </si>
+  <si>
+    <t>Extended value</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Infrastructure and Servers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The servers element describes where the data protected by this data contract is physically located. </t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Catalog</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Delimiter</t>
+  </si>
+  <si>
+    <t>Endpoint URL</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Region Name</t>
+  </si>
+  <si>
+    <t>Databricks Server</t>
+  </si>
+  <si>
+    <t>Azure</t>
+  </si>
+  <si>
+    <t>Amazon Glue</t>
+  </si>
+  <si>
+    <t>Kafka</t>
+  </si>
+  <si>
+    <t>PostgreSQL</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>Snowflake</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>SQL Server</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>Service Name</t>
+  </si>
+  <si>
+    <t>Staging Directory</t>
+  </si>
+  <si>
+    <t>Stream</t>
+  </si>
+  <si>
+    <t>BigQuery</t>
   </si>
 </sst>
 </file>
@@ -642,6 +836,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -660,7 +855,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1386,12 +1580,126 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29635FC6-19E5-6E43-84D3-3161FAC792B3}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="90" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <f>IF(owner &lt;&gt; "", owner, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" sqref="B5:B61" xr:uid="{39D00745-E29F-BB4D-8EFF-9275524C1814}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92ABE851-FB8B-2145-B7F8-5CF6722D55A6}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1475,10 +1783,10 @@
       <c r="B11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="23"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="5"/>
       <c r="E12" s="6"/>
     </row>
@@ -1574,7 +1882,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AK49"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1619,68 +1929,68 @@
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="Y12" s="19" t="s">
@@ -3226,14 +3536,14 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
   </mergeCells>
-  <dataValidations count="11">
+  <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Unique" prompt="A value must be unique within the dataset" sqref="H14:H49" xr:uid="{274C493E-CBE0-2742-BFD6-A161E5736B5A}">
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:C49" xr:uid="{792BC06D-75E6-1A4B-8EE7-26D8A0C4CF46}">
       <formula1>"string,number,integer,boolean,array,object"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" sqref="B14:B49 O14:AK49 J14:J49" xr:uid="{DDC4FF9F-5023-E04B-9FAD-8E0C431863DF}"/>
+    <dataValidation allowBlank="1" sqref="B14:B49 J14:J49 O14:W49 Y14:AK49" xr:uid="{DDC4FF9F-5023-E04B-9FAD-8E0C431863DF}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Required" prompt="Is this a required field (true) or can it be optional (false)" sqref="G14:G49" xr:uid="{653181B6-028C-9348-B6A1-78F7EF7B9A52}">
       <formula1>"true,false"</formula1>
     </dataValidation>
@@ -3250,6 +3560,9 @@
       <formula1>"text,library,sql,custom"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Authoritative Definition URL" prompt="Links to sources that provide more details on the element; examples would be a link to privacy statement, terms and conditions, license agreements, data catalog, or another tool._x000a__x000a_Maps to first authoritativeDefinitions.url_x000a_" sqref="M14:M49" xr:uid="{282580C6-13B6-1B40-9A3A-85842409A299}"/>
+    <dataValidation type="list" allowBlank="1" sqref="X14:X49" xr:uid="{17C32F0F-20AB-664B-ABCA-B45524F93539}">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3656,6 +3969,1058 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B433535-9968-AF4C-822D-F1478F01E2E0}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="59.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" sqref="B5:E61" xr:uid="{87F0D0D6-8894-A64F-B36D-300F6FA120B5}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C18618-CA09-244F-9E12-D5D128AED5CE}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="59.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="32.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="29"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:F4"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" sqref="B7:F63" xr:uid="{7F4EE529-7BE7-6547-817C-8DBC88D35FEC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Schema Name" prompt="The name of the schema (e.g., table) must match the Sheet name &quot;Schema &lt;schema_name&gt;&quot;" sqref="B4:F4" xr:uid="{8220F424-DC29-F648-BD41-E75C77AE8B05}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246082EA-DAAB-1649-871C-B98419509DC8}">
+  <dimension ref="A1:F80"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="36.1640625" style="2" customWidth="1"/>
+    <col min="7" max="22" width="15" style="2" customWidth="1"/>
+    <col min="23" max="30" width="32.83203125" style="2" customWidth="1"/>
+    <col min="31" max="31" width="34.6640625" style="2" customWidth="1"/>
+    <col min="32" max="16384" width="8.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="29"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="7"/>
+      <c r="B18" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+      <c r="B21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="7"/>
+      <c r="B23" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="B26" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="7"/>
+      <c r="B27" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
+      <c r="B28" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="7"/>
+      <c r="B29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="7"/>
+      <c r="B32" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="7"/>
+      <c r="B33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="7"/>
+      <c r="B36" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="7"/>
+      <c r="B38" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="7"/>
+      <c r="B39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="7"/>
+      <c r="B42" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="7"/>
+      <c r="B43" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="7"/>
+      <c r="B44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="7"/>
+      <c r="B45" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="7"/>
+      <c r="B48" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="7"/>
+      <c r="B49" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="7"/>
+      <c r="B50" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="7"/>
+      <c r="B51" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="7"/>
+      <c r="B52" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="7"/>
+      <c r="B53" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="7"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="7"/>
+      <c r="B56" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="7"/>
+      <c r="B57" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="7"/>
+      <c r="B58" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="7"/>
+      <c r="B59" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="7"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="7"/>
+      <c r="B62" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="7"/>
+      <c r="B63" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="7"/>
+      <c r="B64" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="7"/>
+      <c r="B65" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="7"/>
+      <c r="B66" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="7"/>
+      <c r="B67" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="7"/>
+      <c r="B68" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="7"/>
+      <c r="B69" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="7"/>
+      <c r="B70" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="7"/>
+      <c r="B71" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="7"/>
+      <c r="B72" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="7"/>
+      <c r="B73" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="7"/>
+      <c r="B74" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="7"/>
+      <c r="B75" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="7"/>
+      <c r="B76" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="7"/>
+      <c r="B77" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="7"/>
+      <c r="B78" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="7"/>
+      <c r="B79" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="7"/>
+      <c r="B80" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" sqref="G4:AE43 C4:F7 C9:F45 C48:F53 C56:F59 C62:F80" xr:uid="{AEB39A8F-9810-ED4E-9F27-465756D4623D}"/>
+    <dataValidation type="list" allowBlank="1" sqref="C8:F8" xr:uid="{DF709D8D-57D8-6842-9BBE-389F6303D2F1}">
+      <formula1>"api,athena,azure,bigquery,clickhouse,databricks,db2,denodo,dremio,duckdb,glue,cloudsql,informix,kafka,kinesis,mysql,local,oracle,postgresql,presto,pubsub,redshift,s3,sftp,snowflake,sqlserver,synapse,trino,vertica,custom"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95CB51A-C5C4-224E-AA94-69EA1F503FF6}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -3663,9 +5028,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="28" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="28"/>
+    <col min="1" max="1" width="26.1640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="22" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.3">
@@ -3674,7 +5039,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3705,118 +5070,4 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29635FC6-19E5-6E43-84D3-3161FAC792B3}">
-  <dimension ref="A1:B21"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="33.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="90" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <f>IF(owner &lt;&gt; "", owner, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" sqref="B5:B61" xr:uid="{39D00745-E29F-BB4D-8EFF-9275524C1814}"/>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update logical type options
</commit_message>
<xml_diff>
--- a/odcs-template.xlsx
+++ b/odcs-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jochen/Projects/open-data-contract-standard-excel-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150E7A4A-1279-3945-9308-D17E5EF5716B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB6400B-CAF9-9846-A1DC-594202C6C08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2840" yWindow="500" windowWidth="38400" windowHeight="19720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="152">
   <si>
     <t>Property</t>
   </si>
@@ -404,9 +404,6 @@
   </si>
   <si>
     <t>Minimum Properties</t>
-  </si>
-  <si>
-    <t>Required (Object)</t>
   </si>
   <si>
     <t>Pattern</t>
@@ -589,6 +586,15 @@
   </si>
   <si>
     <t>2025-05-05</t>
+  </si>
+  <si>
+    <t>Required Properties</t>
+  </si>
+  <si>
+    <t>Maximum Length</t>
+  </si>
+  <si>
+    <t>Minimum Length</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1412,7 +1418,7 @@
     </row>
     <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -1425,10 +1431,10 @@
     </row>
     <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>143</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>144</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -1441,7 +1447,7 @@
     <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="23"/>
       <c r="B19" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -1464,10 +1470,10 @@
     </row>
     <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>146</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>147</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -1480,7 +1486,7 @@
     <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -1532,7 +1538,7 @@
         <v>39</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
@@ -1896,9 +1902,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AK49"/>
+  <dimension ref="A1:AM49"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1920,26 +1926,26 @@
     <col min="18" max="22" width="19" style="2" customWidth="1"/>
     <col min="23" max="23" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="37" width="21.6640625" style="2" customWidth="1"/>
-    <col min="38" max="16384" width="8.83203125" style="2"/>
+    <col min="25" max="39" width="21.6640625" style="2" customWidth="1"/>
+    <col min="40" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1950,7 +1956,7 @@
       <c r="D5" s="29"/>
       <c r="E5" s="29"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
@@ -1961,7 +1967,7 @@
       <c r="D6" s="29"/>
       <c r="E6" s="29"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -1970,7 +1976,7 @@
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -1979,7 +1985,7 @@
       <c r="D8" s="31"/>
       <c r="E8" s="32"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>53</v>
       </c>
@@ -1988,7 +1994,7 @@
       <c r="D9" s="31"/>
       <c r="E9" s="32"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>54</v>
       </c>
@@ -1997,7 +2003,7 @@
       <c r="D10" s="31"/>
       <c r="E10" s="32"/>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -2006,7 +2012,7 @@
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="Y12" s="19" t="s">
         <v>79</v>
       </c>
@@ -2021,9 +2027,11 @@
       <c r="AH12" s="20"/>
       <c r="AI12" s="20"/>
       <c r="AJ12" s="20"/>
-      <c r="AK12" s="21"/>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AK12" s="20"/>
+      <c r="AL12" s="20"/>
+      <c r="AM12" s="21"/>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>0</v>
       </c>
@@ -2055,10 +2063,10 @@
         <v>13</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M13" s="10" t="s">
         <v>14</v>
@@ -2109,10 +2117,10 @@
         <v>82</v>
       </c>
       <c r="AC13" s="10" t="s">
-        <v>83</v>
+        <v>151</v>
       </c>
       <c r="AD13" s="10" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="AE13" s="10" t="s">
         <v>85</v>
@@ -2121,22 +2129,28 @@
         <v>86</v>
       </c>
       <c r="AG13" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH13" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI13" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="AH13" s="10" t="s">
+      <c r="AJ13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK13" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AI13" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="AJ13" s="10" t="s">
+      <c r="AL13" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="AM13" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="AK13" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -2174,8 +2188,10 @@
       <c r="AI14" s="15"/>
       <c r="AJ14" s="15"/>
       <c r="AK14" s="15"/>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL14" s="15"/>
+      <c r="AM14" s="15"/>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -2213,8 +2229,10 @@
       <c r="AI15" s="15"/>
       <c r="AJ15" s="15"/>
       <c r="AK15" s="15"/>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL15" s="15"/>
+      <c r="AM15" s="15"/>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -2252,8 +2270,10 @@
       <c r="AI16" s="15"/>
       <c r="AJ16" s="15"/>
       <c r="AK16" s="15"/>
-    </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL16" s="15"/>
+      <c r="AM16" s="15"/>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -2291,8 +2311,10 @@
       <c r="AI17" s="15"/>
       <c r="AJ17" s="15"/>
       <c r="AK17" s="15"/>
-    </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL17" s="15"/>
+      <c r="AM17" s="15"/>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -2330,8 +2352,10 @@
       <c r="AI18" s="15"/>
       <c r="AJ18" s="15"/>
       <c r="AK18" s="15"/>
-    </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL18" s="15"/>
+      <c r="AM18" s="15"/>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -2369,8 +2393,10 @@
       <c r="AI19" s="15"/>
       <c r="AJ19" s="15"/>
       <c r="AK19" s="15"/>
-    </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL19" s="15"/>
+      <c r="AM19" s="15"/>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -2408,8 +2434,10 @@
       <c r="AI20" s="15"/>
       <c r="AJ20" s="15"/>
       <c r="AK20" s="15"/>
-    </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL20" s="15"/>
+      <c r="AM20" s="15"/>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
@@ -2447,8 +2475,10 @@
       <c r="AI21" s="15"/>
       <c r="AJ21" s="15"/>
       <c r="AK21" s="15"/>
-    </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL21" s="15"/>
+      <c r="AM21" s="15"/>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -2486,8 +2516,10 @@
       <c r="AI22" s="15"/>
       <c r="AJ22" s="15"/>
       <c r="AK22" s="15"/>
-    </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL22" s="15"/>
+      <c r="AM22" s="15"/>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -2525,8 +2557,10 @@
       <c r="AI23" s="15"/>
       <c r="AJ23" s="15"/>
       <c r="AK23" s="15"/>
-    </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL23" s="15"/>
+      <c r="AM23" s="15"/>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -2564,8 +2598,10 @@
       <c r="AI24" s="15"/>
       <c r="AJ24" s="15"/>
       <c r="AK24" s="15"/>
-    </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL24" s="15"/>
+      <c r="AM24" s="15"/>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -2603,8 +2639,10 @@
       <c r="AI25" s="15"/>
       <c r="AJ25" s="15"/>
       <c r="AK25" s="15"/>
-    </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL25" s="15"/>
+      <c r="AM25" s="15"/>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -2642,8 +2680,10 @@
       <c r="AI26" s="15"/>
       <c r="AJ26" s="15"/>
       <c r="AK26" s="15"/>
-    </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL26" s="15"/>
+      <c r="AM26" s="15"/>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -2681,8 +2721,10 @@
       <c r="AI27" s="15"/>
       <c r="AJ27" s="15"/>
       <c r="AK27" s="15"/>
-    </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL27" s="15"/>
+      <c r="AM27" s="15"/>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -2720,8 +2762,10 @@
       <c r="AI28" s="15"/>
       <c r="AJ28" s="15"/>
       <c r="AK28" s="15"/>
-    </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL28" s="15"/>
+      <c r="AM28" s="15"/>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -2759,8 +2803,10 @@
       <c r="AI29" s="15"/>
       <c r="AJ29" s="15"/>
       <c r="AK29" s="15"/>
-    </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL29" s="15"/>
+      <c r="AM29" s="15"/>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -2798,8 +2844,10 @@
       <c r="AI30" s="15"/>
       <c r="AJ30" s="15"/>
       <c r="AK30" s="15"/>
-    </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL30" s="15"/>
+      <c r="AM30" s="15"/>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -2837,8 +2885,10 @@
       <c r="AI31" s="15"/>
       <c r="AJ31" s="15"/>
       <c r="AK31" s="15"/>
-    </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL31" s="15"/>
+      <c r="AM31" s="15"/>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -2876,8 +2926,10 @@
       <c r="AI32" s="15"/>
       <c r="AJ32" s="15"/>
       <c r="AK32" s="15"/>
-    </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL32" s="15"/>
+      <c r="AM32" s="15"/>
+    </row>
+    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -2915,8 +2967,10 @@
       <c r="AI33" s="15"/>
       <c r="AJ33" s="15"/>
       <c r="AK33" s="15"/>
-    </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL33" s="15"/>
+      <c r="AM33" s="15"/>
+    </row>
+    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -2954,8 +3008,10 @@
       <c r="AI34" s="15"/>
       <c r="AJ34" s="15"/>
       <c r="AK34" s="15"/>
-    </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL34" s="15"/>
+      <c r="AM34" s="15"/>
+    </row>
+    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -2993,8 +3049,10 @@
       <c r="AI35" s="15"/>
       <c r="AJ35" s="15"/>
       <c r="AK35" s="15"/>
-    </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL35" s="15"/>
+      <c r="AM35" s="15"/>
+    </row>
+    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -3032,8 +3090,10 @@
       <c r="AI36" s="15"/>
       <c r="AJ36" s="15"/>
       <c r="AK36" s="15"/>
-    </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL36" s="15"/>
+      <c r="AM36" s="15"/>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -3071,8 +3131,10 @@
       <c r="AI37" s="15"/>
       <c r="AJ37" s="15"/>
       <c r="AK37" s="15"/>
-    </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL37" s="15"/>
+      <c r="AM37" s="15"/>
+    </row>
+    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -3110,8 +3172,10 @@
       <c r="AI38" s="15"/>
       <c r="AJ38" s="15"/>
       <c r="AK38" s="15"/>
-    </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL38" s="15"/>
+      <c r="AM38" s="15"/>
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -3149,8 +3213,10 @@
       <c r="AI39" s="15"/>
       <c r="AJ39" s="15"/>
       <c r="AK39" s="15"/>
-    </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL39" s="15"/>
+      <c r="AM39" s="15"/>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -3188,8 +3254,10 @@
       <c r="AI40" s="15"/>
       <c r="AJ40" s="15"/>
       <c r="AK40" s="15"/>
-    </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL40" s="15"/>
+      <c r="AM40" s="15"/>
+    </row>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -3227,8 +3295,10 @@
       <c r="AI41" s="15"/>
       <c r="AJ41" s="15"/>
       <c r="AK41" s="15"/>
-    </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL41" s="15"/>
+      <c r="AM41" s="15"/>
+    </row>
+    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -3266,8 +3336,10 @@
       <c r="AI42" s="15"/>
       <c r="AJ42" s="15"/>
       <c r="AK42" s="15"/>
-    </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL42" s="15"/>
+      <c r="AM42" s="15"/>
+    </row>
+    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -3305,8 +3377,10 @@
       <c r="AI43" s="15"/>
       <c r="AJ43" s="15"/>
       <c r="AK43" s="15"/>
-    </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL43" s="15"/>
+      <c r="AM43" s="15"/>
+    </row>
+    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -3344,8 +3418,10 @@
       <c r="AI44" s="15"/>
       <c r="AJ44" s="15"/>
       <c r="AK44" s="15"/>
-    </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL44" s="15"/>
+      <c r="AM44" s="15"/>
+    </row>
+    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -3383,8 +3459,10 @@
       <c r="AI45" s="15"/>
       <c r="AJ45" s="15"/>
       <c r="AK45" s="15"/>
-    </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL45" s="15"/>
+      <c r="AM45" s="15"/>
+    </row>
+    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -3422,8 +3500,10 @@
       <c r="AI46" s="15"/>
       <c r="AJ46" s="15"/>
       <c r="AK46" s="15"/>
-    </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL46" s="15"/>
+      <c r="AM46" s="15"/>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -3461,8 +3541,10 @@
       <c r="AI47" s="15"/>
       <c r="AJ47" s="15"/>
       <c r="AK47" s="15"/>
-    </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL47" s="15"/>
+      <c r="AM47" s="15"/>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -3500,8 +3582,10 @@
       <c r="AI48" s="15"/>
       <c r="AJ48" s="15"/>
       <c r="AK48" s="15"/>
-    </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="AL48" s="15"/>
+      <c r="AM48" s="15"/>
+    </row>
+    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -3539,6 +3623,8 @@
       <c r="AI49" s="15"/>
       <c r="AJ49" s="15"/>
       <c r="AK49" s="15"/>
+      <c r="AL49" s="15"/>
+      <c r="AM49" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3557,7 +3643,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:C49" xr:uid="{792BC06D-75E6-1A4B-8EE7-26D8A0C4CF46}">
       <formula1>"string,number,integer,boolean,array,object"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" sqref="B14:B49 J14:J49 O14:W49 Y14:AK49" xr:uid="{DDC4FF9F-5023-E04B-9FAD-8E0C431863DF}"/>
+    <dataValidation allowBlank="1" sqref="B14:B49 J14:J49 O14:W49 AL14:AM49 Y14:AK49" xr:uid="{DDC4FF9F-5023-E04B-9FAD-8E0C431863DF}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Required" prompt="Is this a required field (true) or can it be optional (false)" sqref="G14:G49" xr:uid="{653181B6-028C-9348-B6A1-78F7EF7B9A52}">
       <formula1>"true,false"</formula1>
     </dataValidation>
@@ -4002,12 +4088,12 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -4018,13 +4104,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>102</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -4172,12 +4258,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -4185,7 +4271,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" s="26"/>
     </row>
@@ -4197,16 +4283,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>109</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -4358,9 +4444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246082EA-DAAB-1649-871C-B98419509DC8}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4375,19 +4459,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -4397,7 +4481,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5"/>
@@ -4431,13 +4515,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -4457,7 +4541,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -4469,13 +4553,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -4485,7 +4569,7 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -4497,13 +4581,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -4523,7 +4607,7 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -4535,13 +4619,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -4551,7 +4635,7 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -4561,7 +4645,7 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -4583,13 +4667,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -4611,13 +4695,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -4627,7 +4711,7 @@
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="B37" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -4637,7 +4721,7 @@
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -4659,13 +4743,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -4675,7 +4759,7 @@
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -4695,7 +4779,7 @@
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
       <c r="B45" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -4707,13 +4791,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
       <c r="B48" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -4723,7 +4807,7 @@
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -4733,7 +4817,7 @@
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
       <c r="B50" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -4743,7 +4827,7 @@
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -4753,7 +4837,7 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -4775,13 +4859,13 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
       <c r="B56" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -4791,7 +4875,7 @@
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
       <c r="B57" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -4801,7 +4885,7 @@
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="B58" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -4823,13 +4907,13 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
       <c r="B62" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -4839,7 +4923,7 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
       <c r="B63" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -4849,7 +4933,7 @@
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
       <c r="B64" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -4859,7 +4943,7 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
       <c r="B65" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -4869,7 +4953,7 @@
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
       <c r="B66" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -4879,7 +4963,7 @@
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="7"/>
       <c r="B67" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -4899,7 +4983,7 @@
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
       <c r="B69" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -4909,7 +4993,7 @@
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
       <c r="B70" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -4919,7 +5003,7 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="7"/>
       <c r="B71" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -4929,7 +5013,7 @@
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="7"/>
       <c r="B72" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -4939,7 +5023,7 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="7"/>
       <c r="B73" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
@@ -4949,7 +5033,7 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="7"/>
       <c r="B74" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -4959,7 +5043,7 @@
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="7"/>
       <c r="B75" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
@@ -4979,7 +5063,7 @@
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="7"/>
       <c r="B77" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -4989,7 +5073,7 @@
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="7"/>
       <c r="B78" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -4999,7 +5083,7 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="7"/>
       <c r="B79" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
@@ -5009,7 +5093,7 @@
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="7"/>
       <c r="B80" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
@@ -5042,30 +5126,30 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="5"/>
     </row>
     <row r="5" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="5"/>
     </row>

</xml_diff>

<commit_message>
Added more quality attributes
</commit_message>
<xml_diff>
--- a/odcs-template.xlsx
+++ b/odcs-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jochen/Projects/open-data-contract-standard-excel-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CC8D32-8C2A-3645-8457-E61A038F8459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2164E1-CA7E-264B-9216-856DEED4D844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2840" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
     <definedName name="schema.name" localSheetId="2">'Schema &lt;table_name&gt;'!$B$5</definedName>
     <definedName name="schema.physicalName" localSheetId="2">'Schema &lt;table_name&gt;'!$B$9</definedName>
     <definedName name="schema.physicalType" localSheetId="2">'Schema &lt;table_name&gt;'!$B$6</definedName>
-    <definedName name="schema.properties" localSheetId="2">'Schema &lt;table_name&gt;'!$A$13:$N$981</definedName>
+    <definedName name="schema.properties" localSheetId="2">'Schema &lt;table_name&gt;'!$A$13:$W$981</definedName>
     <definedName name="schema.tags" localSheetId="2">'Schema &lt;table_name&gt;'!$B$11</definedName>
     <definedName name="servers.azure.delimiter">Servers!$C$14</definedName>
     <definedName name="servers.azure.format">Servers!$C$13</definedName>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="162">
   <si>
     <t>Property</t>
   </si>
@@ -598,6 +598,33 @@
   </si>
   <si>
     <t>Existing data contracts with the same ID will be updated.</t>
+  </si>
+  <si>
+    <t>Quality Rule</t>
+  </si>
+  <si>
+    <t>Quality Query</t>
+  </si>
+  <si>
+    <t>Quality Threshold Value</t>
+  </si>
+  <si>
+    <t>Quality Threshold Operator</t>
+  </si>
+  <si>
+    <t>Quality Engine</t>
+  </si>
+  <si>
+    <t>Quality Implementation</t>
+  </si>
+  <si>
+    <t>Quality Severity</t>
+  </si>
+  <si>
+    <t>Quality Scheduler</t>
+  </si>
+  <si>
+    <t>Quality Schedule</t>
   </si>
 </sst>
 </file>
@@ -811,7 +838,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -893,11 +920,99 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3F4F6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3F4F6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3F4F6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3F4F6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3F4F6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3F4F6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3F4F6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3F4F6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3F4F6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1918,7 +2033,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AM49"/>
+  <dimension ref="A1:AV49"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1933,35 +2048,39 @@
     <col min="7" max="8" width="10" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="14.33203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="25.83203125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="28.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.6640625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="19" style="2" customWidth="1"/>
-    <col min="23" max="23" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="39" width="21.6640625" style="2" customWidth="1"/>
-    <col min="40" max="16384" width="8.83203125" style="2"/>
+    <col min="12" max="13" width="25.83203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="29.1640625" style="2" customWidth="1"/>
+    <col min="15" max="16" width="25.83203125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="16.33203125" style="2" customWidth="1"/>
+    <col min="18" max="21" width="25.83203125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="28.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.6640625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="31" width="19" style="2" customWidth="1"/>
+    <col min="32" max="32" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="48" width="21.6640625" style="2" customWidth="1"/>
+    <col min="49" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1972,7 +2091,7 @@
       <c r="D5" s="29"/>
       <c r="E5" s="29"/>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
@@ -1983,7 +2102,7 @@
       <c r="D6" s="29"/>
       <c r="E6" s="29"/>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -1992,7 +2111,7 @@
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -2001,7 +2120,7 @@
       <c r="D8" s="31"/>
       <c r="E8" s="32"/>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>53</v>
       </c>
@@ -2010,7 +2129,7 @@
       <c r="D9" s="31"/>
       <c r="E9" s="32"/>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>54</v>
       </c>
@@ -2019,7 +2138,7 @@
       <c r="D10" s="31"/>
       <c r="E10" s="32"/>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -2028,26 +2147,26 @@
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="Y12" s="19" t="s">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AH12" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="Z12" s="20"/>
-      <c r="AA12" s="20"/>
-      <c r="AB12" s="20"/>
-      <c r="AC12" s="20"/>
-      <c r="AD12" s="20"/>
-      <c r="AE12" s="20"/>
-      <c r="AF12" s="20"/>
-      <c r="AG12" s="20"/>
-      <c r="AH12" s="20"/>
       <c r="AI12" s="20"/>
       <c r="AJ12" s="20"/>
       <c r="AK12" s="20"/>
       <c r="AL12" s="20"/>
-      <c r="AM12" s="21"/>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AM12" s="20"/>
+      <c r="AN12" s="20"/>
+      <c r="AO12" s="20"/>
+      <c r="AP12" s="20"/>
+      <c r="AQ12" s="20"/>
+      <c r="AR12" s="20"/>
+      <c r="AS12" s="20"/>
+      <c r="AT12" s="20"/>
+      <c r="AU12" s="20"/>
+      <c r="AV12" s="21"/>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>0</v>
       </c>
@@ -2085,88 +2204,115 @@
         <v>90</v>
       </c>
       <c r="M13" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="O13" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q13" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="R13" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="S13" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="T13" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="U13" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="V13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="N13" s="10" t="s">
+      <c r="W13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="O13" s="10" t="s">
+      <c r="X13" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="P13" s="10" t="s">
+      <c r="Y13" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="Q13" s="10" t="s">
+      <c r="Z13" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="R13" s="10" t="s">
+      <c r="AA13" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="S13" s="10" t="s">
+      <c r="AB13" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="T13" s="10" t="s">
+      <c r="AC13" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="U13" s="10" t="s">
+      <c r="AD13" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="V13" s="10" t="s">
+      <c r="AE13" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="W13" s="10" t="s">
+      <c r="AF13" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="X13" s="10" t="s">
+      <c r="AG13" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="Y13" s="10" t="s">
+      <c r="AH13" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="Z13" s="10" t="s">
+      <c r="AI13" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="AA13" s="10" t="s">
+      <c r="AJ13" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="AB13" s="10" t="s">
+      <c r="AK13" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="AC13" s="10" t="s">
+      <c r="AL13" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="AD13" s="10" t="s">
+      <c r="AM13" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="AE13" s="10" t="s">
+      <c r="AN13" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="AF13" s="10" t="s">
+      <c r="AO13" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="AG13" s="10" t="s">
+      <c r="AP13" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="AH13" s="10" t="s">
+      <c r="AQ13" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="AI13" s="10" t="s">
+      <c r="AR13" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="AJ13" s="10" t="s">
+      <c r="AS13" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="AK13" s="10" t="s">
+      <c r="AT13" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="AL13" s="10" t="s">
+      <c r="AU13" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="AM13" s="10" t="s">
+      <c r="AV13" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -2206,8 +2352,17 @@
       <c r="AK14" s="15"/>
       <c r="AL14" s="15"/>
       <c r="AM14" s="15"/>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN14" s="15"/>
+      <c r="AO14" s="15"/>
+      <c r="AP14" s="15"/>
+      <c r="AQ14" s="15"/>
+      <c r="AR14" s="15"/>
+      <c r="AS14" s="15"/>
+      <c r="AT14" s="15"/>
+      <c r="AU14" s="15"/>
+      <c r="AV14" s="15"/>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -2221,7 +2376,7 @@
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
+      <c r="N15" s="33"/>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
@@ -2247,8 +2402,17 @@
       <c r="AK15" s="15"/>
       <c r="AL15" s="15"/>
       <c r="AM15" s="15"/>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN15" s="15"/>
+      <c r="AO15" s="15"/>
+      <c r="AP15" s="15"/>
+      <c r="AQ15" s="15"/>
+      <c r="AR15" s="15"/>
+      <c r="AS15" s="15"/>
+      <c r="AT15" s="15"/>
+      <c r="AU15" s="15"/>
+      <c r="AV15" s="15"/>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -2262,7 +2426,7 @@
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
+      <c r="N16" s="33"/>
       <c r="O16" s="15"/>
       <c r="P16" s="15"/>
       <c r="Q16" s="15"/>
@@ -2288,8 +2452,17 @@
       <c r="AK16" s="15"/>
       <c r="AL16" s="15"/>
       <c r="AM16" s="15"/>
-    </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN16" s="15"/>
+      <c r="AO16" s="15"/>
+      <c r="AP16" s="15"/>
+      <c r="AQ16" s="15"/>
+      <c r="AR16" s="15"/>
+      <c r="AS16" s="15"/>
+      <c r="AT16" s="15"/>
+      <c r="AU16" s="15"/>
+      <c r="AV16" s="15"/>
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -2303,7 +2476,7 @@
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
+      <c r="N17" s="33"/>
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
       <c r="Q17" s="15"/>
@@ -2329,8 +2502,17 @@
       <c r="AK17" s="15"/>
       <c r="AL17" s="15"/>
       <c r="AM17" s="15"/>
-    </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN17" s="15"/>
+      <c r="AO17" s="15"/>
+      <c r="AP17" s="15"/>
+      <c r="AQ17" s="15"/>
+      <c r="AR17" s="15"/>
+      <c r="AS17" s="15"/>
+      <c r="AT17" s="15"/>
+      <c r="AU17" s="15"/>
+      <c r="AV17" s="15"/>
+    </row>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -2344,7 +2526,7 @@
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
+      <c r="N18" s="33"/>
       <c r="O18" s="15"/>
       <c r="P18" s="15"/>
       <c r="Q18" s="15"/>
@@ -2370,8 +2552,17 @@
       <c r="AK18" s="15"/>
       <c r="AL18" s="15"/>
       <c r="AM18" s="15"/>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN18" s="15"/>
+      <c r="AO18" s="15"/>
+      <c r="AP18" s="15"/>
+      <c r="AQ18" s="15"/>
+      <c r="AR18" s="15"/>
+      <c r="AS18" s="15"/>
+      <c r="AT18" s="15"/>
+      <c r="AU18" s="15"/>
+      <c r="AV18" s="15"/>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -2385,7 +2576,7 @@
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
+      <c r="N19" s="33"/>
       <c r="O19" s="15"/>
       <c r="P19" s="15"/>
       <c r="Q19" s="15"/>
@@ -2411,8 +2602,17 @@
       <c r="AK19" s="15"/>
       <c r="AL19" s="15"/>
       <c r="AM19" s="15"/>
-    </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN19" s="15"/>
+      <c r="AO19" s="15"/>
+      <c r="AP19" s="15"/>
+      <c r="AQ19" s="15"/>
+      <c r="AR19" s="15"/>
+      <c r="AS19" s="15"/>
+      <c r="AT19" s="15"/>
+      <c r="AU19" s="15"/>
+      <c r="AV19" s="15"/>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -2426,7 +2626,7 @@
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
+      <c r="N20" s="33"/>
       <c r="O20" s="15"/>
       <c r="P20" s="15"/>
       <c r="Q20" s="15"/>
@@ -2452,8 +2652,17 @@
       <c r="AK20" s="15"/>
       <c r="AL20" s="15"/>
       <c r="AM20" s="15"/>
-    </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN20" s="15"/>
+      <c r="AO20" s="15"/>
+      <c r="AP20" s="15"/>
+      <c r="AQ20" s="15"/>
+      <c r="AR20" s="15"/>
+      <c r="AS20" s="15"/>
+      <c r="AT20" s="15"/>
+      <c r="AU20" s="15"/>
+      <c r="AV20" s="15"/>
+    </row>
+    <row r="21" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
@@ -2467,7 +2676,7 @@
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
+      <c r="N21" s="33"/>
       <c r="O21" s="15"/>
       <c r="P21" s="15"/>
       <c r="Q21" s="15"/>
@@ -2493,8 +2702,17 @@
       <c r="AK21" s="15"/>
       <c r="AL21" s="15"/>
       <c r="AM21" s="15"/>
-    </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN21" s="15"/>
+      <c r="AO21" s="15"/>
+      <c r="AP21" s="15"/>
+      <c r="AQ21" s="15"/>
+      <c r="AR21" s="15"/>
+      <c r="AS21" s="15"/>
+      <c r="AT21" s="15"/>
+      <c r="AU21" s="15"/>
+      <c r="AV21" s="15"/>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -2508,7 +2726,7 @@
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
+      <c r="N22" s="33"/>
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
       <c r="Q22" s="15"/>
@@ -2534,8 +2752,17 @@
       <c r="AK22" s="15"/>
       <c r="AL22" s="15"/>
       <c r="AM22" s="15"/>
-    </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN22" s="15"/>
+      <c r="AO22" s="15"/>
+      <c r="AP22" s="15"/>
+      <c r="AQ22" s="15"/>
+      <c r="AR22" s="15"/>
+      <c r="AS22" s="15"/>
+      <c r="AT22" s="15"/>
+      <c r="AU22" s="15"/>
+      <c r="AV22" s="15"/>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -2549,7 +2776,7 @@
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
+      <c r="N23" s="33"/>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
@@ -2575,8 +2802,17 @@
       <c r="AK23" s="15"/>
       <c r="AL23" s="15"/>
       <c r="AM23" s="15"/>
-    </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN23" s="15"/>
+      <c r="AO23" s="15"/>
+      <c r="AP23" s="15"/>
+      <c r="AQ23" s="15"/>
+      <c r="AR23" s="15"/>
+      <c r="AS23" s="15"/>
+      <c r="AT23" s="15"/>
+      <c r="AU23" s="15"/>
+      <c r="AV23" s="15"/>
+    </row>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -2590,7 +2826,7 @@
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="N24" s="33"/>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
@@ -2616,8 +2852,17 @@
       <c r="AK24" s="15"/>
       <c r="AL24" s="15"/>
       <c r="AM24" s="15"/>
-    </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN24" s="15"/>
+      <c r="AO24" s="15"/>
+      <c r="AP24" s="15"/>
+      <c r="AQ24" s="15"/>
+      <c r="AR24" s="15"/>
+      <c r="AS24" s="15"/>
+      <c r="AT24" s="15"/>
+      <c r="AU24" s="15"/>
+      <c r="AV24" s="15"/>
+    </row>
+    <row r="25" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -2631,7 +2876,7 @@
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
       <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
+      <c r="N25" s="33"/>
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
@@ -2657,8 +2902,17 @@
       <c r="AK25" s="15"/>
       <c r="AL25" s="15"/>
       <c r="AM25" s="15"/>
-    </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN25" s="15"/>
+      <c r="AO25" s="15"/>
+      <c r="AP25" s="15"/>
+      <c r="AQ25" s="15"/>
+      <c r="AR25" s="15"/>
+      <c r="AS25" s="15"/>
+      <c r="AT25" s="15"/>
+      <c r="AU25" s="15"/>
+      <c r="AV25" s="15"/>
+    </row>
+    <row r="26" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -2672,7 +2926,7 @@
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
       <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
+      <c r="N26" s="33"/>
       <c r="O26" s="15"/>
       <c r="P26" s="15"/>
       <c r="Q26" s="15"/>
@@ -2698,8 +2952,17 @@
       <c r="AK26" s="15"/>
       <c r="AL26" s="15"/>
       <c r="AM26" s="15"/>
-    </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN26" s="15"/>
+      <c r="AO26" s="15"/>
+      <c r="AP26" s="15"/>
+      <c r="AQ26" s="15"/>
+      <c r="AR26" s="15"/>
+      <c r="AS26" s="15"/>
+      <c r="AT26" s="15"/>
+      <c r="AU26" s="15"/>
+      <c r="AV26" s="15"/>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -2713,7 +2976,7 @@
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
+      <c r="N27" s="33"/>
       <c r="O27" s="15"/>
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
@@ -2739,8 +3002,17 @@
       <c r="AK27" s="15"/>
       <c r="AL27" s="15"/>
       <c r="AM27" s="15"/>
-    </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN27" s="15"/>
+      <c r="AO27" s="15"/>
+      <c r="AP27" s="15"/>
+      <c r="AQ27" s="15"/>
+      <c r="AR27" s="15"/>
+      <c r="AS27" s="15"/>
+      <c r="AT27" s="15"/>
+      <c r="AU27" s="15"/>
+      <c r="AV27" s="15"/>
+    </row>
+    <row r="28" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -2754,7 +3026,7 @@
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
+      <c r="N28" s="33"/>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
@@ -2780,8 +3052,17 @@
       <c r="AK28" s="15"/>
       <c r="AL28" s="15"/>
       <c r="AM28" s="15"/>
-    </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN28" s="15"/>
+      <c r="AO28" s="15"/>
+      <c r="AP28" s="15"/>
+      <c r="AQ28" s="15"/>
+      <c r="AR28" s="15"/>
+      <c r="AS28" s="15"/>
+      <c r="AT28" s="15"/>
+      <c r="AU28" s="15"/>
+      <c r="AV28" s="15"/>
+    </row>
+    <row r="29" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -2795,7 +3076,7 @@
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
       <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
+      <c r="N29" s="33"/>
       <c r="O29" s="15"/>
       <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
@@ -2821,8 +3102,17 @@
       <c r="AK29" s="15"/>
       <c r="AL29" s="15"/>
       <c r="AM29" s="15"/>
-    </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN29" s="15"/>
+      <c r="AO29" s="15"/>
+      <c r="AP29" s="15"/>
+      <c r="AQ29" s="15"/>
+      <c r="AR29" s="15"/>
+      <c r="AS29" s="15"/>
+      <c r="AT29" s="15"/>
+      <c r="AU29" s="15"/>
+      <c r="AV29" s="15"/>
+    </row>
+    <row r="30" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -2836,7 +3126,7 @@
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
+      <c r="N30" s="33"/>
       <c r="O30" s="15"/>
       <c r="P30" s="15"/>
       <c r="Q30" s="15"/>
@@ -2862,8 +3152,17 @@
       <c r="AK30" s="15"/>
       <c r="AL30" s="15"/>
       <c r="AM30" s="15"/>
-    </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN30" s="15"/>
+      <c r="AO30" s="15"/>
+      <c r="AP30" s="15"/>
+      <c r="AQ30" s="15"/>
+      <c r="AR30" s="15"/>
+      <c r="AS30" s="15"/>
+      <c r="AT30" s="15"/>
+      <c r="AU30" s="15"/>
+      <c r="AV30" s="15"/>
+    </row>
+    <row r="31" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -2877,7 +3176,7 @@
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
       <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
+      <c r="N31" s="33"/>
       <c r="O31" s="15"/>
       <c r="P31" s="15"/>
       <c r="Q31" s="15"/>
@@ -2903,8 +3202,17 @@
       <c r="AK31" s="15"/>
       <c r="AL31" s="15"/>
       <c r="AM31" s="15"/>
-    </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN31" s="15"/>
+      <c r="AO31" s="15"/>
+      <c r="AP31" s="15"/>
+      <c r="AQ31" s="15"/>
+      <c r="AR31" s="15"/>
+      <c r="AS31" s="15"/>
+      <c r="AT31" s="15"/>
+      <c r="AU31" s="15"/>
+      <c r="AV31" s="15"/>
+    </row>
+    <row r="32" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -2918,7 +3226,7 @@
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
+      <c r="N32" s="33"/>
       <c r="O32" s="15"/>
       <c r="P32" s="15"/>
       <c r="Q32" s="15"/>
@@ -2944,8 +3252,17 @@
       <c r="AK32" s="15"/>
       <c r="AL32" s="15"/>
       <c r="AM32" s="15"/>
-    </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN32" s="15"/>
+      <c r="AO32" s="15"/>
+      <c r="AP32" s="15"/>
+      <c r="AQ32" s="15"/>
+      <c r="AR32" s="15"/>
+      <c r="AS32" s="15"/>
+      <c r="AT32" s="15"/>
+      <c r="AU32" s="15"/>
+      <c r="AV32" s="15"/>
+    </row>
+    <row r="33" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -2959,7 +3276,7 @@
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
       <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
+      <c r="N33" s="33"/>
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
@@ -2985,8 +3302,17 @@
       <c r="AK33" s="15"/>
       <c r="AL33" s="15"/>
       <c r="AM33" s="15"/>
-    </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN33" s="15"/>
+      <c r="AO33" s="15"/>
+      <c r="AP33" s="15"/>
+      <c r="AQ33" s="15"/>
+      <c r="AR33" s="15"/>
+      <c r="AS33" s="15"/>
+      <c r="AT33" s="15"/>
+      <c r="AU33" s="15"/>
+      <c r="AV33" s="15"/>
+    </row>
+    <row r="34" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -3000,7 +3326,7 @@
       <c r="K34" s="15"/>
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
+      <c r="N34" s="33"/>
       <c r="O34" s="15"/>
       <c r="P34" s="15"/>
       <c r="Q34" s="15"/>
@@ -3026,8 +3352,17 @@
       <c r="AK34" s="15"/>
       <c r="AL34" s="15"/>
       <c r="AM34" s="15"/>
-    </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN34" s="15"/>
+      <c r="AO34" s="15"/>
+      <c r="AP34" s="15"/>
+      <c r="AQ34" s="15"/>
+      <c r="AR34" s="15"/>
+      <c r="AS34" s="15"/>
+      <c r="AT34" s="15"/>
+      <c r="AU34" s="15"/>
+      <c r="AV34" s="15"/>
+    </row>
+    <row r="35" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -3041,7 +3376,7 @@
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
+      <c r="N35" s="33"/>
       <c r="O35" s="15"/>
       <c r="P35" s="15"/>
       <c r="Q35" s="15"/>
@@ -3067,8 +3402,17 @@
       <c r="AK35" s="15"/>
       <c r="AL35" s="15"/>
       <c r="AM35" s="15"/>
-    </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN35" s="15"/>
+      <c r="AO35" s="15"/>
+      <c r="AP35" s="15"/>
+      <c r="AQ35" s="15"/>
+      <c r="AR35" s="15"/>
+      <c r="AS35" s="15"/>
+      <c r="AT35" s="15"/>
+      <c r="AU35" s="15"/>
+      <c r="AV35" s="15"/>
+    </row>
+    <row r="36" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -3082,7 +3426,7 @@
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
+      <c r="N36" s="33"/>
       <c r="O36" s="15"/>
       <c r="P36" s="15"/>
       <c r="Q36" s="15"/>
@@ -3108,8 +3452,17 @@
       <c r="AK36" s="15"/>
       <c r="AL36" s="15"/>
       <c r="AM36" s="15"/>
-    </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN36" s="15"/>
+      <c r="AO36" s="15"/>
+      <c r="AP36" s="15"/>
+      <c r="AQ36" s="15"/>
+      <c r="AR36" s="15"/>
+      <c r="AS36" s="15"/>
+      <c r="AT36" s="15"/>
+      <c r="AU36" s="15"/>
+      <c r="AV36" s="15"/>
+    </row>
+    <row r="37" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -3123,7 +3476,7 @@
       <c r="K37" s="15"/>
       <c r="L37" s="15"/>
       <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
+      <c r="N37" s="33"/>
       <c r="O37" s="15"/>
       <c r="P37" s="15"/>
       <c r="Q37" s="15"/>
@@ -3149,8 +3502,17 @@
       <c r="AK37" s="15"/>
       <c r="AL37" s="15"/>
       <c r="AM37" s="15"/>
-    </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN37" s="15"/>
+      <c r="AO37" s="15"/>
+      <c r="AP37" s="15"/>
+      <c r="AQ37" s="15"/>
+      <c r="AR37" s="15"/>
+      <c r="AS37" s="15"/>
+      <c r="AT37" s="15"/>
+      <c r="AU37" s="15"/>
+      <c r="AV37" s="15"/>
+    </row>
+    <row r="38" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -3164,7 +3526,7 @@
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
+      <c r="N38" s="33"/>
       <c r="O38" s="15"/>
       <c r="P38" s="15"/>
       <c r="Q38" s="15"/>
@@ -3190,8 +3552,17 @@
       <c r="AK38" s="15"/>
       <c r="AL38" s="15"/>
       <c r="AM38" s="15"/>
-    </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN38" s="15"/>
+      <c r="AO38" s="15"/>
+      <c r="AP38" s="15"/>
+      <c r="AQ38" s="15"/>
+      <c r="AR38" s="15"/>
+      <c r="AS38" s="15"/>
+      <c r="AT38" s="15"/>
+      <c r="AU38" s="15"/>
+      <c r="AV38" s="15"/>
+    </row>
+    <row r="39" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -3205,7 +3576,7 @@
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
+      <c r="N39" s="33"/>
       <c r="O39" s="15"/>
       <c r="P39" s="15"/>
       <c r="Q39" s="15"/>
@@ -3231,8 +3602,17 @@
       <c r="AK39" s="15"/>
       <c r="AL39" s="15"/>
       <c r="AM39" s="15"/>
-    </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN39" s="15"/>
+      <c r="AO39" s="15"/>
+      <c r="AP39" s="15"/>
+      <c r="AQ39" s="15"/>
+      <c r="AR39" s="15"/>
+      <c r="AS39" s="15"/>
+      <c r="AT39" s="15"/>
+      <c r="AU39" s="15"/>
+      <c r="AV39" s="15"/>
+    </row>
+    <row r="40" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -3246,7 +3626,7 @@
       <c r="K40" s="15"/>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
+      <c r="N40" s="33"/>
       <c r="O40" s="15"/>
       <c r="P40" s="15"/>
       <c r="Q40" s="15"/>
@@ -3272,8 +3652,17 @@
       <c r="AK40" s="15"/>
       <c r="AL40" s="15"/>
       <c r="AM40" s="15"/>
-    </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN40" s="15"/>
+      <c r="AO40" s="15"/>
+      <c r="AP40" s="15"/>
+      <c r="AQ40" s="15"/>
+      <c r="AR40" s="15"/>
+      <c r="AS40" s="15"/>
+      <c r="AT40" s="15"/>
+      <c r="AU40" s="15"/>
+      <c r="AV40" s="15"/>
+    </row>
+    <row r="41" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -3287,7 +3676,7 @@
       <c r="K41" s="15"/>
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
+      <c r="N41" s="33"/>
       <c r="O41" s="15"/>
       <c r="P41" s="15"/>
       <c r="Q41" s="15"/>
@@ -3313,8 +3702,17 @@
       <c r="AK41" s="15"/>
       <c r="AL41" s="15"/>
       <c r="AM41" s="15"/>
-    </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN41" s="15"/>
+      <c r="AO41" s="15"/>
+      <c r="AP41" s="15"/>
+      <c r="AQ41" s="15"/>
+      <c r="AR41" s="15"/>
+      <c r="AS41" s="15"/>
+      <c r="AT41" s="15"/>
+      <c r="AU41" s="15"/>
+      <c r="AV41" s="15"/>
+    </row>
+    <row r="42" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -3328,7 +3726,7 @@
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
+      <c r="N42" s="33"/>
       <c r="O42" s="15"/>
       <c r="P42" s="15"/>
       <c r="Q42" s="15"/>
@@ -3354,8 +3752,17 @@
       <c r="AK42" s="15"/>
       <c r="AL42" s="15"/>
       <c r="AM42" s="15"/>
-    </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN42" s="15"/>
+      <c r="AO42" s="15"/>
+      <c r="AP42" s="15"/>
+      <c r="AQ42" s="15"/>
+      <c r="AR42" s="15"/>
+      <c r="AS42" s="15"/>
+      <c r="AT42" s="15"/>
+      <c r="AU42" s="15"/>
+      <c r="AV42" s="15"/>
+    </row>
+    <row r="43" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -3369,7 +3776,7 @@
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
+      <c r="N43" s="33"/>
       <c r="O43" s="15"/>
       <c r="P43" s="15"/>
       <c r="Q43" s="15"/>
@@ -3395,8 +3802,17 @@
       <c r="AK43" s="15"/>
       <c r="AL43" s="15"/>
       <c r="AM43" s="15"/>
-    </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN43" s="15"/>
+      <c r="AO43" s="15"/>
+      <c r="AP43" s="15"/>
+      <c r="AQ43" s="15"/>
+      <c r="AR43" s="15"/>
+      <c r="AS43" s="15"/>
+      <c r="AT43" s="15"/>
+      <c r="AU43" s="15"/>
+      <c r="AV43" s="15"/>
+    </row>
+    <row r="44" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -3410,7 +3826,7 @@
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
+      <c r="N44" s="33"/>
       <c r="O44" s="15"/>
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
@@ -3436,8 +3852,17 @@
       <c r="AK44" s="15"/>
       <c r="AL44" s="15"/>
       <c r="AM44" s="15"/>
-    </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN44" s="15"/>
+      <c r="AO44" s="15"/>
+      <c r="AP44" s="15"/>
+      <c r="AQ44" s="15"/>
+      <c r="AR44" s="15"/>
+      <c r="AS44" s="15"/>
+      <c r="AT44" s="15"/>
+      <c r="AU44" s="15"/>
+      <c r="AV44" s="15"/>
+    </row>
+    <row r="45" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -3451,7 +3876,7 @@
       <c r="K45" s="15"/>
       <c r="L45" s="15"/>
       <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
+      <c r="N45" s="33"/>
       <c r="O45" s="15"/>
       <c r="P45" s="15"/>
       <c r="Q45" s="15"/>
@@ -3477,8 +3902,17 @@
       <c r="AK45" s="15"/>
       <c r="AL45" s="15"/>
       <c r="AM45" s="15"/>
-    </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN45" s="15"/>
+      <c r="AO45" s="15"/>
+      <c r="AP45" s="15"/>
+      <c r="AQ45" s="15"/>
+      <c r="AR45" s="15"/>
+      <c r="AS45" s="15"/>
+      <c r="AT45" s="15"/>
+      <c r="AU45" s="15"/>
+      <c r="AV45" s="15"/>
+    </row>
+    <row r="46" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -3492,7 +3926,7 @@
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
+      <c r="N46" s="33"/>
       <c r="O46" s="15"/>
       <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
@@ -3518,8 +3952,17 @@
       <c r="AK46" s="15"/>
       <c r="AL46" s="15"/>
       <c r="AM46" s="15"/>
-    </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN46" s="15"/>
+      <c r="AO46" s="15"/>
+      <c r="AP46" s="15"/>
+      <c r="AQ46" s="15"/>
+      <c r="AR46" s="15"/>
+      <c r="AS46" s="15"/>
+      <c r="AT46" s="15"/>
+      <c r="AU46" s="15"/>
+      <c r="AV46" s="15"/>
+    </row>
+    <row r="47" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -3533,7 +3976,7 @@
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
+      <c r="N47" s="33"/>
       <c r="O47" s="15"/>
       <c r="P47" s="15"/>
       <c r="Q47" s="15"/>
@@ -3559,8 +4002,17 @@
       <c r="AK47" s="15"/>
       <c r="AL47" s="15"/>
       <c r="AM47" s="15"/>
-    </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN47" s="15"/>
+      <c r="AO47" s="15"/>
+      <c r="AP47" s="15"/>
+      <c r="AQ47" s="15"/>
+      <c r="AR47" s="15"/>
+      <c r="AS47" s="15"/>
+      <c r="AT47" s="15"/>
+      <c r="AU47" s="15"/>
+      <c r="AV47" s="15"/>
+    </row>
+    <row r="48" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -3574,7 +4026,7 @@
       <c r="K48" s="15"/>
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
+      <c r="N48" s="33"/>
       <c r="O48" s="15"/>
       <c r="P48" s="15"/>
       <c r="Q48" s="15"/>
@@ -3600,8 +4052,17 @@
       <c r="AK48" s="15"/>
       <c r="AL48" s="15"/>
       <c r="AM48" s="15"/>
-    </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="AN48" s="15"/>
+      <c r="AO48" s="15"/>
+      <c r="AP48" s="15"/>
+      <c r="AQ48" s="15"/>
+      <c r="AR48" s="15"/>
+      <c r="AS48" s="15"/>
+      <c r="AT48" s="15"/>
+      <c r="AU48" s="15"/>
+      <c r="AV48" s="15"/>
+    </row>
+    <row r="49" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -3615,7 +4076,7 @@
       <c r="K49" s="15"/>
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
-      <c r="N49" s="15"/>
+      <c r="N49" s="33"/>
       <c r="O49" s="15"/>
       <c r="P49" s="15"/>
       <c r="Q49" s="15"/>
@@ -3641,6 +4102,15 @@
       <c r="AK49" s="15"/>
       <c r="AL49" s="15"/>
       <c r="AM49" s="15"/>
+      <c r="AN49" s="15"/>
+      <c r="AO49" s="15"/>
+      <c r="AP49" s="15"/>
+      <c r="AQ49" s="15"/>
+      <c r="AR49" s="15"/>
+      <c r="AS49" s="15"/>
+      <c r="AT49" s="15"/>
+      <c r="AU49" s="15"/>
+      <c r="AV49" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3652,21 +4122,31 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
   </mergeCells>
-  <dataValidations count="12">
+  <conditionalFormatting sqref="M14:M9999">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>K14="sql"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N14:N9999">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+      <formula>K14="library"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="22">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Unique" prompt="A value must be unique within the dataset" sqref="H14:H49" xr:uid="{274C493E-CBE0-2742-BFD6-A161E5736B5A}">
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:C49" xr:uid="{792BC06D-75E6-1A4B-8EE7-26D8A0C4CF46}">
       <formula1>"string,number,integer,boolean,array,object"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" sqref="B14:B49 J14:J49 O14:W49 AL14:AM49 Y14:AK49" xr:uid="{DDC4FF9F-5023-E04B-9FAD-8E0C431863DF}"/>
+    <dataValidation allowBlank="1" sqref="B14:B49 J14:J49 X14:AF49 AH14:AV49" xr:uid="{DDC4FF9F-5023-E04B-9FAD-8E0C431863DF}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Required" prompt="Is this a required field (true) or can it be optional (false)" sqref="G14:G49" xr:uid="{653181B6-028C-9348-B6A1-78F7EF7B9A52}">
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality" prompt="The expected or guaranteed data quality from a business perspective._x000a__x000a_Maps to quality.description" sqref="L14:L49" xr:uid="{7B1FC03E-550C-B248-B1C0-23683F595085}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Schema Name" prompt="The name of the schema (e.g., table) must match the Sheet name &quot;Schema &lt;schema_name&gt;&quot;" sqref="B5:E5" xr:uid="{8B3F718D-6361-B845-86DC-2F310C7348A9}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Property" prompt="Name of the property._x000a_If you have structured objects (child properties), use the dot notation, e.g., address.street._x000a_If you have array structures, use the [] notation, e.g., credit_cards[].number." sqref="A13" xr:uid="{0D2C99EC-1C07-E24C-A3B9-1D3DE4A213B3}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Authoritative Definition Type" prompt="Type of definition for authority. Valid values are: businessDefinition, transformationImplementation, videoTutorial, tutorial, and implementation._x000a_ Maps to first authoritativeDefinitions.type_x000a_" sqref="N14:N49" xr:uid="{B83703A8-BFB7-EA4A-8244-28C8F1668E20}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Authoritative Definition Type" prompt="Type of definition for authority. Valid values are: businessDefinition, transformationImplementation, videoTutorial, tutorial, and implementation._x000a_ Maps to first authoritativeDefinitions.type_x000a_" sqref="W14:W49" xr:uid="{B83703A8-BFB7-EA4A-8244-28C8F1668E20}">
       <formula1>"businessDefinition,transformationImplementation,videoTutorial,tutorial,implementation"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="I14:I49" xr:uid="{159197B4-47E7-9F48-923A-42F63EFB1F97}">
@@ -3675,10 +4155,24 @@
     <dataValidation type="list" allowBlank="1" sqref="K14:K49" xr:uid="{B14CC525-9BD9-6A4D-BDFD-7963A22A4F85}">
       <formula1>"text,library,sql,custom"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Authoritative Definition URL" prompt="Links to sources that provide more details on the element; examples would be a link to privacy statement, terms and conditions, license agreements, data catalog, or another tool._x000a__x000a_Maps to first authoritativeDefinitions.url_x000a_" sqref="M14:M49" xr:uid="{282580C6-13B6-1B40-9A3A-85842409A299}"/>
-    <dataValidation type="list" allowBlank="1" sqref="X14:X49" xr:uid="{17C32F0F-20AB-664B-ABCA-B45524F93539}">
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Authoritative Definition URL" prompt="Links to sources that provide more details on the element; examples would be a link to privacy statement, terms and conditions, license agreements, data catalog, or another tool._x000a__x000a_Maps to first authoritativeDefinitions.url_x000a_" sqref="V14:V49" xr:uid="{282580C6-13B6-1B40-9A3A-85842409A299}"/>
+    <dataValidation type="list" allowBlank="1" sqref="AG14:AG49" xr:uid="{17C32F0F-20AB-664B-ABCA-B45524F93539}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Quality Rule" prompt="The expected or guaranteed data quality from a business perspective._x000a__x000a_Maps to quality.description" sqref="M14:M49" xr:uid="{60AD2CA4-9280-D34B-AFCB-2477C280E6E0}">
+      <formula1>"noNullValues,nullValues,noMissingValues,missingValues,noInvalidValues,invalidValues,noDuplicateValues,duplicateValues,freshness"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Query" prompt="A single SQL query that returns either a numeric or boolean value for comparison. The query must be written in the SQL dialect specific to the provided server. " sqref="N14:N49" xr:uid="{723AC735-EE6D-FB49-A65A-FA564073BB7E}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Quality Operator" prompt="The comparation operator specifies the condition to validate the rule._x000a_Use it together with the threshold value, e.g. mustBe 0, or mustBeBetween [0,100]_x000a_This is applicable for quality type sql and some library rules." sqref="O14:O49" xr:uid="{E87C1D95-AE8C-9349-AC4D-E16F3756E552}">
+      <formula1>"mustBe, mustNotBe, mustBeGreaterThan, mustBeGreaterOrEqualTo, mustBeLessThan, mustBeLessOrEqualTo, mustBeBetween, mustNotBeBetween"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Threshold Value" prompt="The acutal value for the treshold operator._x000a_For mustBeBetween adn mustNotBeBetween, use [lowerBoundry, upperBoundy] syntax, e.g. [0, 100]." sqref="P14:P49" xr:uid="{7A30DCB3-38B2-9F4D-B682-91580946AC2A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Engine" prompt="Required for custom DQ rule: name of the third-party engine being used. Any value is authorized here but common values are soda, greatExpectations, montecarlo, etc." sqref="Q14:Q49" xr:uid="{454204BD-5FE9-AA47-BC8C-D830EC5BDE1C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Implementation" prompt="The data quality check in the engine's specific format." sqref="R14:R49" xr:uid="{CB14F0D9-EC9D-8246-9666-65CC45B3A879}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Severity" prompt="The severity of the data quality rule, such as error or warning." sqref="S14:S49" xr:uid="{7388719A-62C1-234E-9F62-FD6D31312CDC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Scheduler" prompt="Name of the scheduler that runs the quality check, such as cron, Airflow, or Github Action." sqref="T14:T49" xr:uid="{D420F1EE-B090-EE4C-A883-DB042581E687}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Schedule Configuration" prompt="Name of the scheduler that runs the quality check, such as cron, Airflow, or Github Action." sqref="U14:U49" xr:uid="{A2DFE74C-1C62-2548-BBA8-044F96FE7A95}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Quality Type" prompt="If you have multiple quality checks for this property, you can copy these columns and add a number, such as &quot;Quality Type 2&quot;, &quot;Quality Description 2&quot;, ..." sqref="K13" xr:uid="{E46F9B9B-5D56-9241-BCB2-51D6C7765942}"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
New sheet for quality, updated logical types.
</commit_message>
<xml_diff>
--- a/odcs-template.xlsx
+++ b/odcs-template.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jochen/Projects/open-data-contract-standard-excel-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2164E1-CA7E-264B-9216-856DEED4D844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DA53B4-0EFF-2648-957B-83AA0B0B88FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="780" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
     <sheet name="Fundamentals" sheetId="10" r:id="rId2"/>
     <sheet name="Schema &lt;table_name&gt;" sheetId="3" r:id="rId3"/>
-    <sheet name="Support" sheetId="12" r:id="rId4"/>
-    <sheet name="Team" sheetId="13" r:id="rId5"/>
-    <sheet name="Roles" sheetId="16" r:id="rId6"/>
-    <sheet name="SLA" sheetId="17" r:id="rId7"/>
-    <sheet name="Servers" sheetId="20" r:id="rId8"/>
-    <sheet name="Pricing" sheetId="15" r:id="rId9"/>
-    <sheet name="Custom Properties" sheetId="11" r:id="rId10"/>
+    <sheet name="Quality" sheetId="21" r:id="rId4"/>
+    <sheet name="Support" sheetId="12" r:id="rId5"/>
+    <sheet name="Team" sheetId="13" r:id="rId6"/>
+    <sheet name="Roles" sheetId="16" r:id="rId7"/>
+    <sheet name="SLA" sheetId="17" r:id="rId8"/>
+    <sheet name="Servers" sheetId="20" r:id="rId9"/>
+    <sheet name="Pricing" sheetId="15" r:id="rId10"/>
+    <sheet name="Custom Properties" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="apiVersion">Fundamentals!$C$5</definedName>
@@ -41,14 +42,14 @@
     <definedName name="price.priceAmount">Pricing!$B$4</definedName>
     <definedName name="price.priceCurrency">Pricing!$B$5</definedName>
     <definedName name="price.priceUnit">Pricing!$B$6</definedName>
-    <definedName name="roles" localSheetId="5">Roles!$A$4:$E$1000</definedName>
+    <definedName name="roles" localSheetId="6">Roles!$A$4:$E$1000</definedName>
     <definedName name="schema.businessName" localSheetId="2">'Schema &lt;table_name&gt;'!$B$8</definedName>
     <definedName name="schema.dataGranularityDescription" localSheetId="2">'Schema &lt;table_name&gt;'!$B$10</definedName>
     <definedName name="schema.description" localSheetId="2">'Schema &lt;table_name&gt;'!$B$7</definedName>
     <definedName name="schema.name" localSheetId="2">'Schema &lt;table_name&gt;'!$B$5</definedName>
     <definedName name="schema.physicalName" localSheetId="2">'Schema &lt;table_name&gt;'!$B$9</definedName>
     <definedName name="schema.physicalType" localSheetId="2">'Schema &lt;table_name&gt;'!$B$6</definedName>
-    <definedName name="schema.properties" localSheetId="2">'Schema &lt;table_name&gt;'!$A$13:$W$981</definedName>
+    <definedName name="schema.properties" localSheetId="2">'Schema &lt;table_name&gt;'!$A$13:$L$981</definedName>
     <definedName name="schema.tags" localSheetId="2">'Schema &lt;table_name&gt;'!$B$11</definedName>
     <definedName name="servers.azure.delimiter">Servers!$C$14</definedName>
     <definedName name="servers.azure.format">Servers!$C$13</definedName>
@@ -105,8 +106,10 @@
     <definedName name="servers.sqlserver.port">Servers!$C$57</definedName>
     <definedName name="servers.sqlserver.schema">Servers!$C$59</definedName>
     <definedName name="servers.type">Servers!$C$8</definedName>
+    <definedName name="slaDefaultElement" localSheetId="3">Quality!#REF!</definedName>
     <definedName name="slaDefaultElement">SLA!$B$4</definedName>
-    <definedName name="slaProperties" localSheetId="6">SLA!$A$6:$F$1002</definedName>
+    <definedName name="slaProperties" localSheetId="3">Quality!$A$4:$G$981</definedName>
+    <definedName name="slaProperties" localSheetId="7">SLA!$A$6:$F$1002</definedName>
     <definedName name="status">Fundamentals!$C$10</definedName>
     <definedName name="support">Support!$A$4:$F$1000</definedName>
     <definedName name="tags">Fundamentals!$C$23</definedName>
@@ -132,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="164">
   <si>
     <t>Property</t>
   </si>
@@ -404,9 +407,6 @@
   </si>
   <si>
     <t>Pattern</t>
-  </si>
-  <si>
-    <t>Quality Description</t>
   </si>
   <si>
     <t>Quality Type</t>
@@ -600,31 +600,40 @@
     <t>Existing data contracts with the same ID will be updated.</t>
   </si>
   <si>
-    <t>Quality Rule</t>
-  </si>
-  <si>
-    <t>Quality Query</t>
-  </si>
-  <si>
-    <t>Quality Threshold Value</t>
-  </si>
-  <si>
-    <t>Quality Threshold Operator</t>
-  </si>
-  <si>
-    <t>Quality Engine</t>
-  </si>
-  <si>
-    <t>Quality Implementation</t>
-  </si>
-  <si>
-    <t>Quality Severity</t>
-  </si>
-  <si>
-    <t>Quality Scheduler</t>
-  </si>
-  <si>
-    <t>Quality Schedule</t>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>This section describes data quality rules &amp; parameters. They are tightly linked to the schema described in the previous sheet(s).</t>
+  </si>
+  <si>
+    <t>Threshold Operator</t>
+  </si>
+  <si>
+    <t>Threshold Value</t>
+  </si>
+  <si>
+    <t>Implementation (Custom)</t>
+  </si>
+  <si>
+    <t>Query (SQL)</t>
+  </si>
+  <si>
+    <t>Quality Engine (Custom)</t>
+  </si>
+  <si>
+    <t>Rule (Library)</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Scheduler</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>Comments (internal)</t>
   </si>
 </sst>
 </file>
@@ -683,7 +692,7 @@
       <name val="Aptos Mono"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -717,6 +726,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCBD5E1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFBEB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -838,7 +853,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -902,6 +917,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -920,14 +938,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -942,80 +960,11 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF3F4F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF3F4F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF3F4F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF3F4F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF3F4F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF3F4F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF3F4F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFBEB"/>
       <color rgb="FFF3F4F6"/>
       <color rgb="FFD1D5DB"/>
       <color rgb="FFCBD5E1"/>
@@ -1536,7 +1485,7 @@
     </row>
     <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -1549,10 +1498,10 @@
     </row>
     <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>141</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>142</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -1565,7 +1514,7 @@
     <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="23"/>
       <c r="B19" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -1588,10 +1537,10 @@
     </row>
     <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -1604,7 +1553,7 @@
     <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="25"/>
       <c r="B22" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -1617,7 +1566,7 @@
     <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -1669,7 +1618,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -1734,6 +1683,58 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95CB51A-C5C4-224E-AA94-69EA1F503FF6}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView zoomScale="165" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.1640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="22" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="5"/>
+    </row>
+  </sheetData>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" sqref="F4:K6" xr:uid="{7EB39568-B879-514E-B51D-6C44C6D6A95F}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29635FC6-19E5-6E43-84D3-3161FAC792B3}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -1936,10 +1937,10 @@
       <c r="B11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="28"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="5"/>
       <c r="E12" s="6"/>
     </row>
@@ -2033,7 +2034,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AV49"/>
+  <dimension ref="A1:AL49"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -2047,126 +2048,122 @@
     <col min="6" max="6" width="35.6640625" style="2" customWidth="1"/>
     <col min="7" max="8" width="10" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="14.33203125" style="2" customWidth="1"/>
-    <col min="12" max="13" width="25.83203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="29.1640625" style="2" customWidth="1"/>
-    <col min="15" max="16" width="25.83203125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="16.33203125" style="2" customWidth="1"/>
-    <col min="18" max="21" width="25.83203125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="28.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28.6640625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="31" width="19" style="2" customWidth="1"/>
-    <col min="32" max="32" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="48" width="21.6640625" style="2" customWidth="1"/>
-    <col min="49" max="16384" width="8.83203125" style="2"/>
+    <col min="10" max="10" width="14.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="28.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="19" style="2" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="37" width="15.5" style="2" customWidth="1"/>
+    <col min="38" max="38" width="26.1640625" style="2" customWidth="1"/>
+    <col min="39" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-    </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-    </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-    </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
-    </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="B8" s="31"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32"/>
-    </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="32"/>
-    </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="B10" s="31"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-    </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="AH12" s="19" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="W12" s="19" t="s">
         <v>79</v>
       </c>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="20"/>
+      <c r="AD12" s="20"/>
+      <c r="AE12" s="20"/>
+      <c r="AF12" s="20"/>
+      <c r="AG12" s="20"/>
+      <c r="AH12" s="20"/>
       <c r="AI12" s="20"/>
       <c r="AJ12" s="20"/>
-      <c r="AK12" s="20"/>
-      <c r="AL12" s="20"/>
-      <c r="AM12" s="20"/>
-      <c r="AN12" s="20"/>
-      <c r="AO12" s="20"/>
-      <c r="AP12" s="20"/>
-      <c r="AQ12" s="20"/>
-      <c r="AR12" s="20"/>
-      <c r="AS12" s="20"/>
-      <c r="AT12" s="20"/>
-      <c r="AU12" s="20"/>
-      <c r="AV12" s="21"/>
-    </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AK12" s="21"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>0</v>
       </c>
@@ -2198,121 +2195,91 @@
         <v>13</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>153</v>
+        <v>53</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>154</v>
+        <v>70</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>156</v>
+        <v>71</v>
       </c>
       <c r="P13" s="10" t="s">
-        <v>155</v>
+        <v>69</v>
       </c>
       <c r="Q13" s="10" t="s">
-        <v>157</v>
+        <v>72</v>
       </c>
       <c r="R13" s="10" t="s">
-        <v>158</v>
+        <v>73</v>
       </c>
       <c r="S13" s="10" t="s">
-        <v>159</v>
+        <v>74</v>
       </c>
       <c r="T13" s="10" t="s">
-        <v>160</v>
+        <v>75</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>161</v>
+        <v>76</v>
       </c>
       <c r="V13" s="10" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="W13" s="10" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
       <c r="X13" s="10" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="Y13" s="10" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="Z13" s="10" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="AA13" s="10" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="AB13" s="10" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="AC13" s="10" t="s">
-        <v>73</v>
+        <v>147</v>
       </c>
       <c r="AD13" s="10" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="AE13" s="10" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="AF13" s="10" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AG13" s="10" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="AH13" s="10" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="AI13" s="10" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="AJ13" s="10" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
       <c r="AK13" s="10" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="AL13" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="AM13" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="AN13" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="AO13" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="AP13" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ13" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR13" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="AS13" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="AT13" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="AU13" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="AV13" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -2350,19 +2317,9 @@
       <c r="AI14" s="15"/>
       <c r="AJ14" s="15"/>
       <c r="AK14" s="15"/>
-      <c r="AL14" s="15"/>
-      <c r="AM14" s="15"/>
-      <c r="AN14" s="15"/>
-      <c r="AO14" s="15"/>
-      <c r="AP14" s="15"/>
-      <c r="AQ14" s="15"/>
-      <c r="AR14" s="15"/>
-      <c r="AS14" s="15"/>
-      <c r="AT14" s="15"/>
-      <c r="AU14" s="15"/>
-      <c r="AV14" s="15"/>
-    </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL14" s="34"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -2376,7 +2333,7 @@
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
-      <c r="N15" s="33"/>
+      <c r="N15" s="15"/>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
@@ -2400,19 +2357,9 @@
       <c r="AI15" s="15"/>
       <c r="AJ15" s="15"/>
       <c r="AK15" s="15"/>
-      <c r="AL15" s="15"/>
-      <c r="AM15" s="15"/>
-      <c r="AN15" s="15"/>
-      <c r="AO15" s="15"/>
-      <c r="AP15" s="15"/>
-      <c r="AQ15" s="15"/>
-      <c r="AR15" s="15"/>
-      <c r="AS15" s="15"/>
-      <c r="AT15" s="15"/>
-      <c r="AU15" s="15"/>
-      <c r="AV15" s="15"/>
-    </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL15" s="34"/>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -2426,7 +2373,7 @@
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
-      <c r="N16" s="33"/>
+      <c r="N16" s="15"/>
       <c r="O16" s="15"/>
       <c r="P16" s="15"/>
       <c r="Q16" s="15"/>
@@ -2450,19 +2397,9 @@
       <c r="AI16" s="15"/>
       <c r="AJ16" s="15"/>
       <c r="AK16" s="15"/>
-      <c r="AL16" s="15"/>
-      <c r="AM16" s="15"/>
-      <c r="AN16" s="15"/>
-      <c r="AO16" s="15"/>
-      <c r="AP16" s="15"/>
-      <c r="AQ16" s="15"/>
-      <c r="AR16" s="15"/>
-      <c r="AS16" s="15"/>
-      <c r="AT16" s="15"/>
-      <c r="AU16" s="15"/>
-      <c r="AV16" s="15"/>
-    </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL16" s="34"/>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A17" s="17"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -2476,7 +2413,7 @@
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
-      <c r="N17" s="33"/>
+      <c r="N17" s="15"/>
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
       <c r="Q17" s="15"/>
@@ -2500,19 +2437,9 @@
       <c r="AI17" s="15"/>
       <c r="AJ17" s="15"/>
       <c r="AK17" s="15"/>
-      <c r="AL17" s="15"/>
-      <c r="AM17" s="15"/>
-      <c r="AN17" s="15"/>
-      <c r="AO17" s="15"/>
-      <c r="AP17" s="15"/>
-      <c r="AQ17" s="15"/>
-      <c r="AR17" s="15"/>
-      <c r="AS17" s="15"/>
-      <c r="AT17" s="15"/>
-      <c r="AU17" s="15"/>
-      <c r="AV17" s="15"/>
-    </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL17" s="34"/>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -2526,7 +2453,7 @@
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
-      <c r="N18" s="33"/>
+      <c r="N18" s="15"/>
       <c r="O18" s="15"/>
       <c r="P18" s="15"/>
       <c r="Q18" s="15"/>
@@ -2550,19 +2477,9 @@
       <c r="AI18" s="15"/>
       <c r="AJ18" s="15"/>
       <c r="AK18" s="15"/>
-      <c r="AL18" s="15"/>
-      <c r="AM18" s="15"/>
-      <c r="AN18" s="15"/>
-      <c r="AO18" s="15"/>
-      <c r="AP18" s="15"/>
-      <c r="AQ18" s="15"/>
-      <c r="AR18" s="15"/>
-      <c r="AS18" s="15"/>
-      <c r="AT18" s="15"/>
-      <c r="AU18" s="15"/>
-      <c r="AV18" s="15"/>
-    </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL18" s="34"/>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -2576,7 +2493,7 @@
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
-      <c r="N19" s="33"/>
+      <c r="N19" s="15"/>
       <c r="O19" s="15"/>
       <c r="P19" s="15"/>
       <c r="Q19" s="15"/>
@@ -2600,19 +2517,9 @@
       <c r="AI19" s="15"/>
       <c r="AJ19" s="15"/>
       <c r="AK19" s="15"/>
-      <c r="AL19" s="15"/>
-      <c r="AM19" s="15"/>
-      <c r="AN19" s="15"/>
-      <c r="AO19" s="15"/>
-      <c r="AP19" s="15"/>
-      <c r="AQ19" s="15"/>
-      <c r="AR19" s="15"/>
-      <c r="AS19" s="15"/>
-      <c r="AT19" s="15"/>
-      <c r="AU19" s="15"/>
-      <c r="AV19" s="15"/>
-    </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL19" s="34"/>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -2626,7 +2533,7 @@
       <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
-      <c r="N20" s="33"/>
+      <c r="N20" s="15"/>
       <c r="O20" s="15"/>
       <c r="P20" s="15"/>
       <c r="Q20" s="15"/>
@@ -2650,19 +2557,9 @@
       <c r="AI20" s="15"/>
       <c r="AJ20" s="15"/>
       <c r="AK20" s="15"/>
-      <c r="AL20" s="15"/>
-      <c r="AM20" s="15"/>
-      <c r="AN20" s="15"/>
-      <c r="AO20" s="15"/>
-      <c r="AP20" s="15"/>
-      <c r="AQ20" s="15"/>
-      <c r="AR20" s="15"/>
-      <c r="AS20" s="15"/>
-      <c r="AT20" s="15"/>
-      <c r="AU20" s="15"/>
-      <c r="AV20" s="15"/>
-    </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL20" s="34"/>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
@@ -2676,7 +2573,7 @@
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
-      <c r="N21" s="33"/>
+      <c r="N21" s="15"/>
       <c r="O21" s="15"/>
       <c r="P21" s="15"/>
       <c r="Q21" s="15"/>
@@ -2700,19 +2597,9 @@
       <c r="AI21" s="15"/>
       <c r="AJ21" s="15"/>
       <c r="AK21" s="15"/>
-      <c r="AL21" s="15"/>
-      <c r="AM21" s="15"/>
-      <c r="AN21" s="15"/>
-      <c r="AO21" s="15"/>
-      <c r="AP21" s="15"/>
-      <c r="AQ21" s="15"/>
-      <c r="AR21" s="15"/>
-      <c r="AS21" s="15"/>
-      <c r="AT21" s="15"/>
-      <c r="AU21" s="15"/>
-      <c r="AV21" s="15"/>
-    </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL21" s="34"/>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -2726,7 +2613,7 @@
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
-      <c r="N22" s="33"/>
+      <c r="N22" s="15"/>
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
       <c r="Q22" s="15"/>
@@ -2750,19 +2637,9 @@
       <c r="AI22" s="15"/>
       <c r="AJ22" s="15"/>
       <c r="AK22" s="15"/>
-      <c r="AL22" s="15"/>
-      <c r="AM22" s="15"/>
-      <c r="AN22" s="15"/>
-      <c r="AO22" s="15"/>
-      <c r="AP22" s="15"/>
-      <c r="AQ22" s="15"/>
-      <c r="AR22" s="15"/>
-      <c r="AS22" s="15"/>
-      <c r="AT22" s="15"/>
-      <c r="AU22" s="15"/>
-      <c r="AV22" s="15"/>
-    </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL22" s="34"/>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -2776,7 +2653,7 @@
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
-      <c r="N23" s="33"/>
+      <c r="N23" s="15"/>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
@@ -2800,19 +2677,9 @@
       <c r="AI23" s="15"/>
       <c r="AJ23" s="15"/>
       <c r="AK23" s="15"/>
-      <c r="AL23" s="15"/>
-      <c r="AM23" s="15"/>
-      <c r="AN23" s="15"/>
-      <c r="AO23" s="15"/>
-      <c r="AP23" s="15"/>
-      <c r="AQ23" s="15"/>
-      <c r="AR23" s="15"/>
-      <c r="AS23" s="15"/>
-      <c r="AT23" s="15"/>
-      <c r="AU23" s="15"/>
-      <c r="AV23" s="15"/>
-    </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL23" s="34"/>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -2826,7 +2693,7 @@
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
-      <c r="N24" s="33"/>
+      <c r="N24" s="15"/>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
@@ -2850,19 +2717,9 @@
       <c r="AI24" s="15"/>
       <c r="AJ24" s="15"/>
       <c r="AK24" s="15"/>
-      <c r="AL24" s="15"/>
-      <c r="AM24" s="15"/>
-      <c r="AN24" s="15"/>
-      <c r="AO24" s="15"/>
-      <c r="AP24" s="15"/>
-      <c r="AQ24" s="15"/>
-      <c r="AR24" s="15"/>
-      <c r="AS24" s="15"/>
-      <c r="AT24" s="15"/>
-      <c r="AU24" s="15"/>
-      <c r="AV24" s="15"/>
-    </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL24" s="34"/>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -2876,7 +2733,7 @@
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
       <c r="M25" s="15"/>
-      <c r="N25" s="33"/>
+      <c r="N25" s="15"/>
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
@@ -2900,19 +2757,9 @@
       <c r="AI25" s="15"/>
       <c r="AJ25" s="15"/>
       <c r="AK25" s="15"/>
-      <c r="AL25" s="15"/>
-      <c r="AM25" s="15"/>
-      <c r="AN25" s="15"/>
-      <c r="AO25" s="15"/>
-      <c r="AP25" s="15"/>
-      <c r="AQ25" s="15"/>
-      <c r="AR25" s="15"/>
-      <c r="AS25" s="15"/>
-      <c r="AT25" s="15"/>
-      <c r="AU25" s="15"/>
-      <c r="AV25" s="15"/>
-    </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL25" s="34"/>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A26" s="17"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -2926,7 +2773,7 @@
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
       <c r="M26" s="15"/>
-      <c r="N26" s="33"/>
+      <c r="N26" s="15"/>
       <c r="O26" s="15"/>
       <c r="P26" s="15"/>
       <c r="Q26" s="15"/>
@@ -2950,19 +2797,9 @@
       <c r="AI26" s="15"/>
       <c r="AJ26" s="15"/>
       <c r="AK26" s="15"/>
-      <c r="AL26" s="15"/>
-      <c r="AM26" s="15"/>
-      <c r="AN26" s="15"/>
-      <c r="AO26" s="15"/>
-      <c r="AP26" s="15"/>
-      <c r="AQ26" s="15"/>
-      <c r="AR26" s="15"/>
-      <c r="AS26" s="15"/>
-      <c r="AT26" s="15"/>
-      <c r="AU26" s="15"/>
-      <c r="AV26" s="15"/>
-    </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL26" s="34"/>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A27" s="17"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -2976,7 +2813,7 @@
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
-      <c r="N27" s="33"/>
+      <c r="N27" s="15"/>
       <c r="O27" s="15"/>
       <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
@@ -3000,19 +2837,9 @@
       <c r="AI27" s="15"/>
       <c r="AJ27" s="15"/>
       <c r="AK27" s="15"/>
-      <c r="AL27" s="15"/>
-      <c r="AM27" s="15"/>
-      <c r="AN27" s="15"/>
-      <c r="AO27" s="15"/>
-      <c r="AP27" s="15"/>
-      <c r="AQ27" s="15"/>
-      <c r="AR27" s="15"/>
-      <c r="AS27" s="15"/>
-      <c r="AT27" s="15"/>
-      <c r="AU27" s="15"/>
-      <c r="AV27" s="15"/>
-    </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL27" s="34"/>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A28" s="17"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -3026,7 +2853,7 @@
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
-      <c r="N28" s="33"/>
+      <c r="N28" s="15"/>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
@@ -3050,19 +2877,9 @@
       <c r="AI28" s="15"/>
       <c r="AJ28" s="15"/>
       <c r="AK28" s="15"/>
-      <c r="AL28" s="15"/>
-      <c r="AM28" s="15"/>
-      <c r="AN28" s="15"/>
-      <c r="AO28" s="15"/>
-      <c r="AP28" s="15"/>
-      <c r="AQ28" s="15"/>
-      <c r="AR28" s="15"/>
-      <c r="AS28" s="15"/>
-      <c r="AT28" s="15"/>
-      <c r="AU28" s="15"/>
-      <c r="AV28" s="15"/>
-    </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL28" s="34"/>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -3076,7 +2893,7 @@
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
       <c r="M29" s="15"/>
-      <c r="N29" s="33"/>
+      <c r="N29" s="15"/>
       <c r="O29" s="15"/>
       <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
@@ -3100,19 +2917,9 @@
       <c r="AI29" s="15"/>
       <c r="AJ29" s="15"/>
       <c r="AK29" s="15"/>
-      <c r="AL29" s="15"/>
-      <c r="AM29" s="15"/>
-      <c r="AN29" s="15"/>
-      <c r="AO29" s="15"/>
-      <c r="AP29" s="15"/>
-      <c r="AQ29" s="15"/>
-      <c r="AR29" s="15"/>
-      <c r="AS29" s="15"/>
-      <c r="AT29" s="15"/>
-      <c r="AU29" s="15"/>
-      <c r="AV29" s="15"/>
-    </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL29" s="34"/>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -3126,7 +2933,7 @@
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
-      <c r="N30" s="33"/>
+      <c r="N30" s="15"/>
       <c r="O30" s="15"/>
       <c r="P30" s="15"/>
       <c r="Q30" s="15"/>
@@ -3150,19 +2957,9 @@
       <c r="AI30" s="15"/>
       <c r="AJ30" s="15"/>
       <c r="AK30" s="15"/>
-      <c r="AL30" s="15"/>
-      <c r="AM30" s="15"/>
-      <c r="AN30" s="15"/>
-      <c r="AO30" s="15"/>
-      <c r="AP30" s="15"/>
-      <c r="AQ30" s="15"/>
-      <c r="AR30" s="15"/>
-      <c r="AS30" s="15"/>
-      <c r="AT30" s="15"/>
-      <c r="AU30" s="15"/>
-      <c r="AV30" s="15"/>
-    </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL30" s="34"/>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -3176,7 +2973,7 @@
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
       <c r="M31" s="15"/>
-      <c r="N31" s="33"/>
+      <c r="N31" s="15"/>
       <c r="O31" s="15"/>
       <c r="P31" s="15"/>
       <c r="Q31" s="15"/>
@@ -3200,19 +2997,9 @@
       <c r="AI31" s="15"/>
       <c r="AJ31" s="15"/>
       <c r="AK31" s="15"/>
-      <c r="AL31" s="15"/>
-      <c r="AM31" s="15"/>
-      <c r="AN31" s="15"/>
-      <c r="AO31" s="15"/>
-      <c r="AP31" s="15"/>
-      <c r="AQ31" s="15"/>
-      <c r="AR31" s="15"/>
-      <c r="AS31" s="15"/>
-      <c r="AT31" s="15"/>
-      <c r="AU31" s="15"/>
-      <c r="AV31" s="15"/>
-    </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL31" s="34"/>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A32" s="17"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -3226,7 +3013,7 @@
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
-      <c r="N32" s="33"/>
+      <c r="N32" s="15"/>
       <c r="O32" s="15"/>
       <c r="P32" s="15"/>
       <c r="Q32" s="15"/>
@@ -3250,19 +3037,9 @@
       <c r="AI32" s="15"/>
       <c r="AJ32" s="15"/>
       <c r="AK32" s="15"/>
-      <c r="AL32" s="15"/>
-      <c r="AM32" s="15"/>
-      <c r="AN32" s="15"/>
-      <c r="AO32" s="15"/>
-      <c r="AP32" s="15"/>
-      <c r="AQ32" s="15"/>
-      <c r="AR32" s="15"/>
-      <c r="AS32" s="15"/>
-      <c r="AT32" s="15"/>
-      <c r="AU32" s="15"/>
-      <c r="AV32" s="15"/>
-    </row>
-    <row r="33" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL32" s="34"/>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A33" s="17"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -3276,7 +3053,7 @@
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
       <c r="M33" s="15"/>
-      <c r="N33" s="33"/>
+      <c r="N33" s="15"/>
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
@@ -3300,19 +3077,9 @@
       <c r="AI33" s="15"/>
       <c r="AJ33" s="15"/>
       <c r="AK33" s="15"/>
-      <c r="AL33" s="15"/>
-      <c r="AM33" s="15"/>
-      <c r="AN33" s="15"/>
-      <c r="AO33" s="15"/>
-      <c r="AP33" s="15"/>
-      <c r="AQ33" s="15"/>
-      <c r="AR33" s="15"/>
-      <c r="AS33" s="15"/>
-      <c r="AT33" s="15"/>
-      <c r="AU33" s="15"/>
-      <c r="AV33" s="15"/>
-    </row>
-    <row r="34" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL33" s="34"/>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A34" s="17"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -3326,7 +3093,7 @@
       <c r="K34" s="15"/>
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
-      <c r="N34" s="33"/>
+      <c r="N34" s="15"/>
       <c r="O34" s="15"/>
       <c r="P34" s="15"/>
       <c r="Q34" s="15"/>
@@ -3350,19 +3117,9 @@
       <c r="AI34" s="15"/>
       <c r="AJ34" s="15"/>
       <c r="AK34" s="15"/>
-      <c r="AL34" s="15"/>
-      <c r="AM34" s="15"/>
-      <c r="AN34" s="15"/>
-      <c r="AO34" s="15"/>
-      <c r="AP34" s="15"/>
-      <c r="AQ34" s="15"/>
-      <c r="AR34" s="15"/>
-      <c r="AS34" s="15"/>
-      <c r="AT34" s="15"/>
-      <c r="AU34" s="15"/>
-      <c r="AV34" s="15"/>
-    </row>
-    <row r="35" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL34" s="34"/>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A35" s="17"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -3376,7 +3133,7 @@
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
-      <c r="N35" s="33"/>
+      <c r="N35" s="15"/>
       <c r="O35" s="15"/>
       <c r="P35" s="15"/>
       <c r="Q35" s="15"/>
@@ -3400,19 +3157,9 @@
       <c r="AI35" s="15"/>
       <c r="AJ35" s="15"/>
       <c r="AK35" s="15"/>
-      <c r="AL35" s="15"/>
-      <c r="AM35" s="15"/>
-      <c r="AN35" s="15"/>
-      <c r="AO35" s="15"/>
-      <c r="AP35" s="15"/>
-      <c r="AQ35" s="15"/>
-      <c r="AR35" s="15"/>
-      <c r="AS35" s="15"/>
-      <c r="AT35" s="15"/>
-      <c r="AU35" s="15"/>
-      <c r="AV35" s="15"/>
-    </row>
-    <row r="36" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL35" s="34"/>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A36" s="17"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -3426,7 +3173,7 @@
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
-      <c r="N36" s="33"/>
+      <c r="N36" s="15"/>
       <c r="O36" s="15"/>
       <c r="P36" s="15"/>
       <c r="Q36" s="15"/>
@@ -3450,19 +3197,9 @@
       <c r="AI36" s="15"/>
       <c r="AJ36" s="15"/>
       <c r="AK36" s="15"/>
-      <c r="AL36" s="15"/>
-      <c r="AM36" s="15"/>
-      <c r="AN36" s="15"/>
-      <c r="AO36" s="15"/>
-      <c r="AP36" s="15"/>
-      <c r="AQ36" s="15"/>
-      <c r="AR36" s="15"/>
-      <c r="AS36" s="15"/>
-      <c r="AT36" s="15"/>
-      <c r="AU36" s="15"/>
-      <c r="AV36" s="15"/>
-    </row>
-    <row r="37" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL36" s="34"/>
+    </row>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A37" s="17"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -3476,7 +3213,7 @@
       <c r="K37" s="15"/>
       <c r="L37" s="15"/>
       <c r="M37" s="15"/>
-      <c r="N37" s="33"/>
+      <c r="N37" s="15"/>
       <c r="O37" s="15"/>
       <c r="P37" s="15"/>
       <c r="Q37" s="15"/>
@@ -3500,19 +3237,9 @@
       <c r="AI37" s="15"/>
       <c r="AJ37" s="15"/>
       <c r="AK37" s="15"/>
-      <c r="AL37" s="15"/>
-      <c r="AM37" s="15"/>
-      <c r="AN37" s="15"/>
-      <c r="AO37" s="15"/>
-      <c r="AP37" s="15"/>
-      <c r="AQ37" s="15"/>
-      <c r="AR37" s="15"/>
-      <c r="AS37" s="15"/>
-      <c r="AT37" s="15"/>
-      <c r="AU37" s="15"/>
-      <c r="AV37" s="15"/>
-    </row>
-    <row r="38" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL37" s="34"/>
+    </row>
+    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A38" s="17"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -3526,7 +3253,7 @@
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
-      <c r="N38" s="33"/>
+      <c r="N38" s="15"/>
       <c r="O38" s="15"/>
       <c r="P38" s="15"/>
       <c r="Q38" s="15"/>
@@ -3550,19 +3277,9 @@
       <c r="AI38" s="15"/>
       <c r="AJ38" s="15"/>
       <c r="AK38" s="15"/>
-      <c r="AL38" s="15"/>
-      <c r="AM38" s="15"/>
-      <c r="AN38" s="15"/>
-      <c r="AO38" s="15"/>
-      <c r="AP38" s="15"/>
-      <c r="AQ38" s="15"/>
-      <c r="AR38" s="15"/>
-      <c r="AS38" s="15"/>
-      <c r="AT38" s="15"/>
-      <c r="AU38" s="15"/>
-      <c r="AV38" s="15"/>
-    </row>
-    <row r="39" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL38" s="34"/>
+    </row>
+    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A39" s="17"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -3576,7 +3293,7 @@
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
-      <c r="N39" s="33"/>
+      <c r="N39" s="15"/>
       <c r="O39" s="15"/>
       <c r="P39" s="15"/>
       <c r="Q39" s="15"/>
@@ -3600,19 +3317,9 @@
       <c r="AI39" s="15"/>
       <c r="AJ39" s="15"/>
       <c r="AK39" s="15"/>
-      <c r="AL39" s="15"/>
-      <c r="AM39" s="15"/>
-      <c r="AN39" s="15"/>
-      <c r="AO39" s="15"/>
-      <c r="AP39" s="15"/>
-      <c r="AQ39" s="15"/>
-      <c r="AR39" s="15"/>
-      <c r="AS39" s="15"/>
-      <c r="AT39" s="15"/>
-      <c r="AU39" s="15"/>
-      <c r="AV39" s="15"/>
-    </row>
-    <row r="40" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL39" s="34"/>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A40" s="17"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -3626,7 +3333,7 @@
       <c r="K40" s="15"/>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
-      <c r="N40" s="33"/>
+      <c r="N40" s="15"/>
       <c r="O40" s="15"/>
       <c r="P40" s="15"/>
       <c r="Q40" s="15"/>
@@ -3650,19 +3357,9 @@
       <c r="AI40" s="15"/>
       <c r="AJ40" s="15"/>
       <c r="AK40" s="15"/>
-      <c r="AL40" s="15"/>
-      <c r="AM40" s="15"/>
-      <c r="AN40" s="15"/>
-      <c r="AO40" s="15"/>
-      <c r="AP40" s="15"/>
-      <c r="AQ40" s="15"/>
-      <c r="AR40" s="15"/>
-      <c r="AS40" s="15"/>
-      <c r="AT40" s="15"/>
-      <c r="AU40" s="15"/>
-      <c r="AV40" s="15"/>
-    </row>
-    <row r="41" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL40" s="34"/>
+    </row>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A41" s="17"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -3676,7 +3373,7 @@
       <c r="K41" s="15"/>
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
-      <c r="N41" s="33"/>
+      <c r="N41" s="15"/>
       <c r="O41" s="15"/>
       <c r="P41" s="15"/>
       <c r="Q41" s="15"/>
@@ -3700,19 +3397,9 @@
       <c r="AI41" s="15"/>
       <c r="AJ41" s="15"/>
       <c r="AK41" s="15"/>
-      <c r="AL41" s="15"/>
-      <c r="AM41" s="15"/>
-      <c r="AN41" s="15"/>
-      <c r="AO41" s="15"/>
-      <c r="AP41" s="15"/>
-      <c r="AQ41" s="15"/>
-      <c r="AR41" s="15"/>
-      <c r="AS41" s="15"/>
-      <c r="AT41" s="15"/>
-      <c r="AU41" s="15"/>
-      <c r="AV41" s="15"/>
-    </row>
-    <row r="42" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL41" s="34"/>
+    </row>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A42" s="17"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -3726,7 +3413,7 @@
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
-      <c r="N42" s="33"/>
+      <c r="N42" s="15"/>
       <c r="O42" s="15"/>
       <c r="P42" s="15"/>
       <c r="Q42" s="15"/>
@@ -3750,19 +3437,9 @@
       <c r="AI42" s="15"/>
       <c r="AJ42" s="15"/>
       <c r="AK42" s="15"/>
-      <c r="AL42" s="15"/>
-      <c r="AM42" s="15"/>
-      <c r="AN42" s="15"/>
-      <c r="AO42" s="15"/>
-      <c r="AP42" s="15"/>
-      <c r="AQ42" s="15"/>
-      <c r="AR42" s="15"/>
-      <c r="AS42" s="15"/>
-      <c r="AT42" s="15"/>
-      <c r="AU42" s="15"/>
-      <c r="AV42" s="15"/>
-    </row>
-    <row r="43" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL42" s="34"/>
+    </row>
+    <row r="43" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A43" s="17"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -3776,7 +3453,7 @@
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
-      <c r="N43" s="33"/>
+      <c r="N43" s="15"/>
       <c r="O43" s="15"/>
       <c r="P43" s="15"/>
       <c r="Q43" s="15"/>
@@ -3800,19 +3477,9 @@
       <c r="AI43" s="15"/>
       <c r="AJ43" s="15"/>
       <c r="AK43" s="15"/>
-      <c r="AL43" s="15"/>
-      <c r="AM43" s="15"/>
-      <c r="AN43" s="15"/>
-      <c r="AO43" s="15"/>
-      <c r="AP43" s="15"/>
-      <c r="AQ43" s="15"/>
-      <c r="AR43" s="15"/>
-      <c r="AS43" s="15"/>
-      <c r="AT43" s="15"/>
-      <c r="AU43" s="15"/>
-      <c r="AV43" s="15"/>
-    </row>
-    <row r="44" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL43" s="34"/>
+    </row>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A44" s="17"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -3826,7 +3493,7 @@
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
-      <c r="N44" s="33"/>
+      <c r="N44" s="15"/>
       <c r="O44" s="15"/>
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
@@ -3850,19 +3517,9 @@
       <c r="AI44" s="15"/>
       <c r="AJ44" s="15"/>
       <c r="AK44" s="15"/>
-      <c r="AL44" s="15"/>
-      <c r="AM44" s="15"/>
-      <c r="AN44" s="15"/>
-      <c r="AO44" s="15"/>
-      <c r="AP44" s="15"/>
-      <c r="AQ44" s="15"/>
-      <c r="AR44" s="15"/>
-      <c r="AS44" s="15"/>
-      <c r="AT44" s="15"/>
-      <c r="AU44" s="15"/>
-      <c r="AV44" s="15"/>
-    </row>
-    <row r="45" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL44" s="34"/>
+    </row>
+    <row r="45" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A45" s="17"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -3876,7 +3533,7 @@
       <c r="K45" s="15"/>
       <c r="L45" s="15"/>
       <c r="M45" s="15"/>
-      <c r="N45" s="33"/>
+      <c r="N45" s="15"/>
       <c r="O45" s="15"/>
       <c r="P45" s="15"/>
       <c r="Q45" s="15"/>
@@ -3900,19 +3557,9 @@
       <c r="AI45" s="15"/>
       <c r="AJ45" s="15"/>
       <c r="AK45" s="15"/>
-      <c r="AL45" s="15"/>
-      <c r="AM45" s="15"/>
-      <c r="AN45" s="15"/>
-      <c r="AO45" s="15"/>
-      <c r="AP45" s="15"/>
-      <c r="AQ45" s="15"/>
-      <c r="AR45" s="15"/>
-      <c r="AS45" s="15"/>
-      <c r="AT45" s="15"/>
-      <c r="AU45" s="15"/>
-      <c r="AV45" s="15"/>
-    </row>
-    <row r="46" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL45" s="34"/>
+    </row>
+    <row r="46" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A46" s="17"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -3926,7 +3573,7 @@
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
-      <c r="N46" s="33"/>
+      <c r="N46" s="15"/>
       <c r="O46" s="15"/>
       <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
@@ -3950,19 +3597,9 @@
       <c r="AI46" s="15"/>
       <c r="AJ46" s="15"/>
       <c r="AK46" s="15"/>
-      <c r="AL46" s="15"/>
-      <c r="AM46" s="15"/>
-      <c r="AN46" s="15"/>
-      <c r="AO46" s="15"/>
-      <c r="AP46" s="15"/>
-      <c r="AQ46" s="15"/>
-      <c r="AR46" s="15"/>
-      <c r="AS46" s="15"/>
-      <c r="AT46" s="15"/>
-      <c r="AU46" s="15"/>
-      <c r="AV46" s="15"/>
-    </row>
-    <row r="47" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL46" s="34"/>
+    </row>
+    <row r="47" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -3976,7 +3613,7 @@
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
-      <c r="N47" s="33"/>
+      <c r="N47" s="15"/>
       <c r="O47" s="15"/>
       <c r="P47" s="15"/>
       <c r="Q47" s="15"/>
@@ -4000,19 +3637,9 @@
       <c r="AI47" s="15"/>
       <c r="AJ47" s="15"/>
       <c r="AK47" s="15"/>
-      <c r="AL47" s="15"/>
-      <c r="AM47" s="15"/>
-      <c r="AN47" s="15"/>
-      <c r="AO47" s="15"/>
-      <c r="AP47" s="15"/>
-      <c r="AQ47" s="15"/>
-      <c r="AR47" s="15"/>
-      <c r="AS47" s="15"/>
-      <c r="AT47" s="15"/>
-      <c r="AU47" s="15"/>
-      <c r="AV47" s="15"/>
-    </row>
-    <row r="48" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL47" s="34"/>
+    </row>
+    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A48" s="17"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -4026,7 +3653,7 @@
       <c r="K48" s="15"/>
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
-      <c r="N48" s="33"/>
+      <c r="N48" s="15"/>
       <c r="O48" s="15"/>
       <c r="P48" s="15"/>
       <c r="Q48" s="15"/>
@@ -4050,19 +3677,9 @@
       <c r="AI48" s="15"/>
       <c r="AJ48" s="15"/>
       <c r="AK48" s="15"/>
-      <c r="AL48" s="15"/>
-      <c r="AM48" s="15"/>
-      <c r="AN48" s="15"/>
-      <c r="AO48" s="15"/>
-      <c r="AP48" s="15"/>
-      <c r="AQ48" s="15"/>
-      <c r="AR48" s="15"/>
-      <c r="AS48" s="15"/>
-      <c r="AT48" s="15"/>
-      <c r="AU48" s="15"/>
-      <c r="AV48" s="15"/>
-    </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="AL48" s="34"/>
+    </row>
+    <row r="49" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -4076,7 +3693,7 @@
       <c r="K49" s="15"/>
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
-      <c r="N49" s="33"/>
+      <c r="N49" s="15"/>
       <c r="O49" s="15"/>
       <c r="P49" s="15"/>
       <c r="Q49" s="15"/>
@@ -4100,17 +3717,7 @@
       <c r="AI49" s="15"/>
       <c r="AJ49" s="15"/>
       <c r="AK49" s="15"/>
-      <c r="AL49" s="15"/>
-      <c r="AM49" s="15"/>
-      <c r="AN49" s="15"/>
-      <c r="AO49" s="15"/>
-      <c r="AP49" s="15"/>
-      <c r="AQ49" s="15"/>
-      <c r="AR49" s="15"/>
-      <c r="AS49" s="15"/>
-      <c r="AT49" s="15"/>
-      <c r="AU49" s="15"/>
-      <c r="AV49" s="15"/>
+      <c r="AL49" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4122,63 +3729,412 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
   </mergeCells>
-  <conditionalFormatting sqref="M14:M9999">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
-      <formula>K14="sql"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N14:N9999">
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
-      <formula>K14="library"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="22">
+  <dataValidations count="11">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Unique" prompt="A value must be unique within the dataset" sqref="H14:H49" xr:uid="{274C493E-CBE0-2742-BFD6-A161E5736B5A}">
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:C49" xr:uid="{792BC06D-75E6-1A4B-8EE7-26D8A0C4CF46}">
-      <formula1>"string,number,integer,boolean,array,object"</formula1>
+      <formula1>"string,number,integer,boolean,array,object,timestamp,date,time"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" sqref="B14:B49 J14:J49 X14:AF49 AH14:AV49" xr:uid="{DDC4FF9F-5023-E04B-9FAD-8E0C431863DF}"/>
+    <dataValidation allowBlank="1" sqref="B14:B49 J14:J49 M14:U49 W14:AL49" xr:uid="{DDC4FF9F-5023-E04B-9FAD-8E0C431863DF}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Required" prompt="Is this a required field (true) or can it be optional (false)" sqref="G14:G49" xr:uid="{653181B6-028C-9348-B6A1-78F7EF7B9A52}">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality" prompt="The expected or guaranteed data quality from a business perspective._x000a__x000a_Maps to quality.description" sqref="L14:L49" xr:uid="{7B1FC03E-550C-B248-B1C0-23683F595085}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Schema Name" prompt="The name of the schema (e.g., table) must match the Sheet name &quot;Schema &lt;schema_name&gt;&quot;" sqref="B5:E5" xr:uid="{8B3F718D-6361-B845-86DC-2F310C7348A9}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Property" prompt="Name of the property._x000a_If you have structured objects (child properties), use the dot notation, e.g., address.street._x000a_If you have array structures, use the [] notation, e.g., credit_cards[].number." sqref="A13" xr:uid="{0D2C99EC-1C07-E24C-A3B9-1D3DE4A213B3}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Authoritative Definition Type" prompt="Type of definition for authority. Valid values are: businessDefinition, transformationImplementation, videoTutorial, tutorial, and implementation._x000a_ Maps to first authoritativeDefinitions.type_x000a_" sqref="W14:W49" xr:uid="{B83703A8-BFB7-EA4A-8244-28C8F1668E20}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Authoritative Definition Type" prompt="Type of definition for authority. Valid values are: businessDefinition, transformationImplementation, videoTutorial, tutorial, and implementation._x000a_ Maps to first authoritativeDefinitions.type_x000a_" sqref="L14:L49" xr:uid="{B83703A8-BFB7-EA4A-8244-28C8F1668E20}">
       <formula1>"businessDefinition,transformationImplementation,videoTutorial,tutorial,implementation"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="I14:I49" xr:uid="{159197B4-47E7-9F48-923A-42F63EFB1F97}">
       <formula1>"confidential,restricted,public"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="K14:K49" xr:uid="{B14CC525-9BD9-6A4D-BDFD-7963A22A4F85}">
-      <formula1>"text,library,sql,custom"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Authoritative Definition URL" prompt="Links to sources that provide more details on the element; examples would be a link to privacy statement, terms and conditions, license agreements, data catalog, or another tool._x000a__x000a_Maps to first authoritativeDefinitions.url_x000a_" sqref="V14:V49" xr:uid="{282580C6-13B6-1B40-9A3A-85842409A299}"/>
-    <dataValidation type="list" allowBlank="1" sqref="AG14:AG49" xr:uid="{17C32F0F-20AB-664B-ABCA-B45524F93539}">
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Authoritative Definition URL" prompt="Links to sources that provide more details on the element; examples would be a link to privacy statement, terms and conditions, license agreements, data catalog, or another tool._x000a__x000a_Maps to first authoritativeDefinitions.url_x000a_" sqref="K14:K49" xr:uid="{282580C6-13B6-1B40-9A3A-85842409A299}"/>
+    <dataValidation type="list" allowBlank="1" sqref="V14:V49" xr:uid="{17C32F0F-20AB-664B-ABCA-B45524F93539}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Quality Rule" prompt="The expected or guaranteed data quality from a business perspective._x000a__x000a_Maps to quality.description" sqref="M14:M49" xr:uid="{60AD2CA4-9280-D34B-AFCB-2477C280E6E0}">
-      <formula1>"noNullValues,nullValues,noMissingValues,missingValues,noInvalidValues,invalidValues,noDuplicateValues,duplicateValues,freshness"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Query" prompt="A single SQL query that returns either a numeric or boolean value for comparison. The query must be written in the SQL dialect specific to the provided server. " sqref="N14:N49" xr:uid="{723AC735-EE6D-FB49-A65A-FA564073BB7E}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Quality Operator" prompt="The comparation operator specifies the condition to validate the rule._x000a_Use it together with the threshold value, e.g. mustBe 0, or mustBeBetween [0,100]_x000a_This is applicable for quality type sql and some library rules." sqref="O14:O49" xr:uid="{E87C1D95-AE8C-9349-AC4D-E16F3756E552}">
-      <formula1>"mustBe, mustNotBe, mustBeGreaterThan, mustBeGreaterOrEqualTo, mustBeLessThan, mustBeLessOrEqualTo, mustBeBetween, mustNotBeBetween"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Threshold Value" prompt="The acutal value for the treshold operator._x000a_For mustBeBetween adn mustNotBeBetween, use [lowerBoundry, upperBoundy] syntax, e.g. [0, 100]." sqref="P14:P49" xr:uid="{7A30DCB3-38B2-9F4D-B682-91580946AC2A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Engine" prompt="Required for custom DQ rule: name of the third-party engine being used. Any value is authorized here but common values are soda, greatExpectations, montecarlo, etc." sqref="Q14:Q49" xr:uid="{454204BD-5FE9-AA47-BC8C-D830EC5BDE1C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Implementation" prompt="The data quality check in the engine's specific format." sqref="R14:R49" xr:uid="{CB14F0D9-EC9D-8246-9666-65CC45B3A879}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Severity" prompt="The severity of the data quality rule, such as error or warning." sqref="S14:S49" xr:uid="{7388719A-62C1-234E-9F62-FD6D31312CDC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Scheduler" prompt="Name of the scheduler that runs the quality check, such as cron, Airflow, or Github Action." sqref="T14:T49" xr:uid="{D420F1EE-B090-EE4C-A883-DB042581E687}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Schedule Configuration" prompt="Name of the scheduler that runs the quality check, such as cron, Airflow, or Github Action." sqref="U14:U49" xr:uid="{A2DFE74C-1C62-2548-BBA8-044F96FE7A95}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Quality Type" prompt="If you have multiple quality checks for this property, you can copy these columns and add a number, such as &quot;Quality Type 2&quot;, &quot;Quality Description 2&quot;, ..." sqref="K13" xr:uid="{E46F9B9B-5D56-9241-BCB2-51D6C7765942}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Comments" prompt="Use this for internal comments, open questions, discussion points. _x000a_This will not become part of the ODCS YAML." sqref="AL13" xr:uid="{D669647A-617C-7549-9EA2-AC37BFEA6E41}"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0F4C5A-BE41-6140-9B9B-80B8DB7D1AD7}">
+  <dimension ref="A1:M21"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" style="2" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E5:E21">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>C5="sql"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:F21">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+      <formula>C5="library"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="15">
+    <dataValidation allowBlank="1" sqref="C22:G42" xr:uid="{E994B14B-32F5-D346-A2D5-4948CC9EA8C3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Quality Type" prompt="Data quality rules support different levels/stages of data quality attributes:_x000a__x000a_Text: A human-readable text that describes the quality of the data._x000a_Library rules: A maintained library of commonly-used predefined quality attributes such as rowCount, unique" sqref="C4" xr:uid="{F5034942-1DBE-6649-8226-7716B942E17B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Scheduler" prompt="Name of the scheduler that runs the quality check, such as cron, Airflow, or Github Action." sqref="L5:M21" xr:uid="{32CE7D0C-23F9-9242-8EB2-22364F11133E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Severity" prompt="The severity of the data quality rule, such as error or warning." sqref="K5:K21" xr:uid="{0F4D661D-23D9-2540-B241-435A8E49610F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Implementation" prompt="The data quality check in the engine's specific format." sqref="J5:J21" xr:uid="{00416CE8-FD1E-374C-B0CF-0FDCB1952802}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Engine" prompt="Required for custom DQ rule: name of the third-party engine being used. Any value is authorized here but common values are soda, greatExpectations, montecarlo, etc." sqref="I5:I21" xr:uid="{0459F568-8532-4048-9CA7-5708CD6DF179}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Threshold Value" prompt="The acutal value for the treshold operator._x000a_For mustBeBetween adn mustNotBeBetween, use [lowerBoundry, upperBoundy] syntax, e.g. [0, 100]." sqref="H5:H21" xr:uid="{E792E24E-6B57-A948-A026-4637119AD944}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Quality Operator" prompt="The comparation operator specifies the condition to validate the rule._x000a_Use it together with the threshold value, e.g. mustBe 0, or mustBeBetween [0,100]_x000a_This is applicable for quality type sql and some library rules." sqref="G5:G21" xr:uid="{15B1EE74-8A6D-3F49-A7EC-55C27203D116}">
+      <formula1>"mustBe, mustNotBe, mustBeGreaterThan, mustBeGreaterOrEqualTo, mustBeLessThan, mustBeLessOrEqualTo, mustBeBetween, mustNotBeBetween"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality Query" prompt="A single SQL query that returns either a numeric or boolean value for comparison. The query must be written in the SQL dialect specific to the provided server. " sqref="F5:F21" xr:uid="{21D55077-EE2C-364C-A32A-00F4CC049BEA}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Quality Rule" prompt="The expected or guaranteed data quality from a business perspective._x000a__x000a_Maps to quality.description" sqref="E5:E21" xr:uid="{FA04105D-EE78-664F-8C72-4098B271EC60}">
+      <formula1>"noNullValues,nullValues,noMissingValues,missingValues,noInvalidValues,invalidValues,noDuplicateValues,duplicateValues,freshness"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C5:C21" xr:uid="{664F88A2-7556-9B4E-A851-8889D6576B99}">
+      <formula1>"text,library,sql,custom"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Quality" prompt="The expected or guaranteed data quality from a business perspective._x000a__x000a_Maps to quality.description" sqref="D5:D21" xr:uid="{C84C6FF8-FC8D-B848-AC69-3DB82C6CB871}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Schema" prompt="The schema name must match the name of the schema (table, ...) in the previous sheets." sqref="A4" xr:uid="{67CAE90D-676C-A44B-B965-361A399ACA9A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Property" prompt="Optional: Leave empty, if this is a schema-level quality check._x000a_The property must match the property name in the schema._x000a_" sqref="B4" xr:uid="{F3E67713-E117-6E46-AEFE-6861F5933838}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Rule" prompt="The predefined data quality rule from the library._x000a_Only appliable if &quot;Quality Type&quot; is set to &quot;library&quot; or empty (which is library by default, if a rule is defined)" sqref="E4" xr:uid="{4E8AA24F-1E70-FF4C-81CC-D9A25B05246C}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90FB3633-F435-1B44-A99B-F400ACF77C57}">
   <dimension ref="A1:F21"/>
   <sheetViews>
@@ -4368,7 +4324,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD55E6DF-E5C5-C142-BA93-791862A30BE7}">
   <dimension ref="A1:G21"/>
   <sheetViews>
@@ -4578,7 +4534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B433535-9968-AF4C-822D-F1478F01E2E0}">
   <dimension ref="A1:E21"/>
   <sheetViews>
@@ -4598,12 +4554,12 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -4614,13 +4570,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>100</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -4750,7 +4706,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C18618-CA09-244F-9E12-D5D128AED5CE}">
   <dimension ref="A1:F23"/>
   <sheetViews>
@@ -4768,12 +4724,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -4781,7 +4737,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="26"/>
     </row>
@@ -4793,16 +4749,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>107</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -4950,7 +4906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246082EA-DAAB-1649-871C-B98419509DC8}">
   <dimension ref="A1:F80"/>
   <sheetViews>
@@ -4969,19 +4925,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -4991,7 +4947,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="5"/>
@@ -5025,13 +4981,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -5051,7 +5007,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -5063,13 +5019,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -5079,7 +5035,7 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -5091,13 +5047,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -5117,7 +5073,7 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -5129,13 +5085,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -5145,7 +5101,7 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -5155,7 +5111,7 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -5177,13 +5133,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -5205,13 +5161,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -5221,7 +5177,7 @@
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="B37" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -5231,7 +5187,7 @@
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -5253,13 +5209,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -5269,7 +5225,7 @@
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -5289,7 +5245,7 @@
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
       <c r="B45" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -5301,13 +5257,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
       <c r="B48" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -5317,7 +5273,7 @@
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -5327,7 +5283,7 @@
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
       <c r="B50" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -5337,7 +5293,7 @@
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -5347,7 +5303,7 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -5369,13 +5325,13 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
       <c r="B56" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -5385,7 +5341,7 @@
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
       <c r="B57" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -5395,7 +5351,7 @@
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="B58" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -5417,13 +5373,13 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
       <c r="B62" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -5433,7 +5389,7 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
       <c r="B63" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -5443,7 +5399,7 @@
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
       <c r="B64" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -5453,7 +5409,7 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
       <c r="B65" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -5463,7 +5419,7 @@
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
       <c r="B66" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -5473,7 +5429,7 @@
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="7"/>
       <c r="B67" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -5493,7 +5449,7 @@
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
       <c r="B69" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -5503,7 +5459,7 @@
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
       <c r="B70" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -5513,7 +5469,7 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="7"/>
       <c r="B71" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -5523,7 +5479,7 @@
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="7"/>
       <c r="B72" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -5533,7 +5489,7 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="7"/>
       <c r="B73" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
@@ -5543,7 +5499,7 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="7"/>
       <c r="B74" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -5553,7 +5509,7 @@
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="7"/>
       <c r="B75" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
@@ -5573,7 +5529,7 @@
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="7"/>
       <c r="B77" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -5583,7 +5539,7 @@
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="7"/>
       <c r="B78" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -5593,7 +5549,7 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="7"/>
       <c r="B79" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
@@ -5603,7 +5559,7 @@
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="7"/>
       <c r="B80" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
@@ -5619,56 +5575,4 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95CB51A-C5C4-224E-AA94-69EA1F503FF6}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView zoomScale="165" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26.1640625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="22" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="22"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="5"/>
-    </row>
-  </sheetData>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" sqref="F4:K6" xr:uid="{7EB39568-B879-514E-B51D-6C44C6D6A95F}">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>